<commit_message>
KDV teklif listesine eklendi
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SIRA</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>FIYAT</t>
+  </si>
+  <si>
+    <t>KDV</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G2" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +380,10 @@
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="85.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,6 +403,9 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mail gönderdeki button slindi
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7640"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;TL&quot;_-;\-* #,##0.00\ &quot;TL&quot;_-;_-* &quot;-&quot;??\ &quot;TL&quot;_-;_-@_-"/>
   </numFmts>
@@ -179,7 +179,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -208,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,23 +494,23 @@
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="59.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="6" width="59.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="E1" s="8"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -517,7 +518,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -527,7 +528,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -535,13 +536,13 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F5" s="15" t="s">
         <v>12</v>
       </c>
@@ -550,7 +551,7 @@
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +584,7 @@
       </c>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E8" s="9"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -591,15 +592,15 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -607,7 +608,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -615,7 +616,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -623,7 +624,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -631,7 +632,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -639,7 +640,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -647,7 +648,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -655,7 +656,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -663,7 +664,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -671,7 +672,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -679,7 +680,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -687,7 +688,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -695,7 +696,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E22" s="9"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -703,7 +704,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -711,7 +712,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E24" s="9"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -719,7 +720,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -727,7 +728,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -735,7 +736,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -743,7 +744,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E28" s="9"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -751,7 +752,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -759,7 +760,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E30" s="9"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -767,7 +768,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -775,7 +776,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -783,7 +784,7 @@
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -791,7 +792,7 @@
       <c r="I33" s="11"/>
       <c r="J33" s="12"/>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -799,7 +800,7 @@
       <c r="I34" s="11"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E35" s="9"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -807,7 +808,7 @@
       <c r="I35" s="11"/>
       <c r="J35" s="12"/>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -815,7 +816,7 @@
       <c r="I36" s="11"/>
       <c r="J36" s="12"/>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E37" s="9"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -823,7 +824,7 @@
       <c r="I37" s="11"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -831,7 +832,7 @@
       <c r="I38" s="11"/>
       <c r="J38" s="12"/>
     </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -839,7 +840,7 @@
       <c r="I39" s="11"/>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
@@ -847,7 +848,7 @@
       <c r="I40" s="11"/>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E41" s="9"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -855,7 +856,7 @@
       <c r="I41" s="11"/>
       <c r="J41" s="12"/>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
@@ -863,7 +864,7 @@
       <c r="I42" s="11"/>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E43" s="9"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -871,7 +872,7 @@
       <c r="I43" s="11"/>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E44" s="9"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -879,7 +880,7 @@
       <c r="I44" s="11"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -887,7 +888,7 @@
       <c r="I45" s="11"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
@@ -895,7 +896,7 @@
       <c r="I46" s="11"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
@@ -903,7 +904,7 @@
       <c r="I47" s="11"/>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
@@ -911,7 +912,7 @@
       <c r="I48" s="11"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E49" s="9"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
@@ -919,7 +920,7 @@
       <c r="I49" s="11"/>
       <c r="J49" s="12"/>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E50" s="9"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
@@ -927,7 +928,7 @@
       <c r="I50" s="11"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E51" s="9"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
@@ -935,7 +936,7 @@
       <c r="I51" s="11"/>
       <c r="J51" s="12"/>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E52" s="9"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
@@ -943,7 +944,7 @@
       <c r="I52" s="11"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E53" s="9"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -951,7 +952,7 @@
       <c r="I53" s="11"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E54" s="9"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
@@ -959,7 +960,7 @@
       <c r="I54" s="11"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E55" s="9"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
@@ -967,7 +968,7 @@
       <c r="I55" s="11"/>
       <c r="J55" s="12"/>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E56" s="9"/>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
@@ -975,7 +976,7 @@
       <c r="I56" s="11"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E57" s="9"/>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>

</xml_diff>

<commit_message>
Kuzen ufak tefek birkaç güncelleme yaptım 27.02.2018
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -57,14 +57,17 @@
     <t>Tarih:</t>
   </si>
   <si>
-    <t>Aşağıdaki tabloda belirtilen malzemeler için KDV hariç teklif fyatlarınızı bekler; Hayırlı çalışmalar dileriz.</t>
+    <t>Aşağıdaki tabloda belirtilen malzemeler için KDV hariç teklif fiyatlarınızı bekler; Hayırlı çalışmalar dileriz.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;TL&quot;_-;\-* #,##0.00\ &quot;TL&quot;_-;_-* &quot;-&quot;??\ &quot;TL&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +127,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -164,10 +174,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -181,14 +193,19 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ParaBirimi" xfId="1" builtinId="4"/>
+    <cellStyle name="Yüzde" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,13 +535,13 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -539,25 +556,1569 @@
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="14"/>
+    </row>
+    <row r="86" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="14"/>
+    </row>
+    <row r="89" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="14"/>
+    </row>
+    <row r="90" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="14"/>
+    </row>
+    <row r="91" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="14"/>
+    </row>
+    <row r="93" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="14"/>
+    </row>
+    <row r="94" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="14"/>
+    </row>
+    <row r="95" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="14"/>
+    </row>
+    <row r="97" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="14"/>
+    </row>
+    <row r="99" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="14"/>
+    </row>
+    <row r="100" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="14"/>
+    </row>
+    <row r="101" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="14"/>
+    </row>
+    <row r="102" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="14"/>
+    </row>
+    <row r="103" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="14"/>
+    </row>
+    <row r="104" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="14"/>
+    </row>
+    <row r="105" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="14"/>
+    </row>
+    <row r="106" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="12"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="14"/>
+    </row>
+    <row r="107" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="12"/>
+      <c r="H108" s="12"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="14"/>
+    </row>
+    <row r="109" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="12"/>
+      <c r="H109" s="12"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="12"/>
+      <c r="H110" s="12"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="14"/>
+    </row>
+    <row r="112" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="14"/>
+    </row>
+    <row r="113" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="12"/>
+      <c r="H114" s="12"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="12"/>
+      <c r="H115" s="12"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+      <c r="G116" s="12"/>
+      <c r="H116" s="12"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="14"/>
+    </row>
+    <row r="117" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="14"/>
+    </row>
+    <row r="119" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="14"/>
+    </row>
+    <row r="120" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="14"/>
+    </row>
+    <row r="121" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="14"/>
+    </row>
+    <row r="122" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="14"/>
+    </row>
+    <row r="123" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="12"/>
+      <c r="H123" s="12"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="14"/>
+    </row>
+    <row r="124" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+      <c r="G124" s="12"/>
+      <c r="H124" s="12"/>
+      <c r="I124" s="13"/>
+      <c r="J124" s="14"/>
+    </row>
+    <row r="125" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="12"/>
+      <c r="H125" s="12"/>
+      <c r="I125" s="13"/>
+      <c r="J125" s="14"/>
+    </row>
+    <row r="126" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+      <c r="I126" s="13"/>
+      <c r="J126" s="14"/>
+    </row>
+    <row r="127" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="14"/>
+    </row>
+    <row r="128" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+      <c r="G128" s="12"/>
+      <c r="H128" s="12"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="14"/>
+    </row>
+    <row r="129" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+      <c r="G129" s="12"/>
+      <c r="H129" s="12"/>
+      <c r="I129" s="13"/>
+      <c r="J129" s="14"/>
+    </row>
+    <row r="130" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
+      <c r="I130" s="13"/>
+      <c r="J130" s="14"/>
+    </row>
+    <row r="131" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+      <c r="G131" s="12"/>
+      <c r="H131" s="12"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="14"/>
+    </row>
+    <row r="132" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="14"/>
+    </row>
+    <row r="133" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+      <c r="I133" s="13"/>
+      <c r="J133" s="14"/>
+    </row>
+    <row r="134" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="12"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="14"/>
+    </row>
+    <row r="135" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="14"/>
+    </row>
+    <row r="136" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="14"/>
+    </row>
+    <row r="137" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="14"/>
+    </row>
+    <row r="138" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="13"/>
+      <c r="J138" s="14"/>
+    </row>
+    <row r="139" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="13"/>
+      <c r="J139" s="14"/>
+    </row>
+    <row r="140" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="12"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="14"/>
+    </row>
+    <row r="141" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E141" s="12"/>
+      <c r="F141" s="12"/>
+      <c r="G141" s="12"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="13"/>
+      <c r="J141" s="14"/>
+    </row>
+    <row r="142" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E142" s="12"/>
+      <c r="F142" s="12"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="14"/>
+    </row>
+    <row r="143" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
+      <c r="G143" s="12"/>
+      <c r="H143" s="12"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="14"/>
+    </row>
+    <row r="144" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E144" s="12"/>
+      <c r="F144" s="12"/>
+      <c r="G144" s="12"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="14"/>
+    </row>
+    <row r="145" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E145" s="12"/>
+      <c r="F145" s="12"/>
+      <c r="G145" s="12"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="14"/>
+    </row>
+    <row r="146" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E146" s="12"/>
+      <c r="F146" s="12"/>
+      <c r="G146" s="12"/>
+      <c r="H146" s="12"/>
+      <c r="I146" s="13"/>
+      <c r="J146" s="14"/>
+    </row>
+    <row r="147" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E147" s="12"/>
+      <c r="F147" s="12"/>
+      <c r="G147" s="12"/>
+      <c r="H147" s="12"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="14"/>
+    </row>
+    <row r="148" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E148" s="12"/>
+      <c r="F148" s="12"/>
+      <c r="G148" s="12"/>
+      <c r="H148" s="12"/>
+      <c r="I148" s="13"/>
+      <c r="J148" s="14"/>
+    </row>
+    <row r="149" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E149" s="12"/>
+      <c r="F149" s="12"/>
+      <c r="G149" s="12"/>
+      <c r="H149" s="12"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="14"/>
+    </row>
+    <row r="150" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E150" s="12"/>
+      <c r="F150" s="12"/>
+      <c r="G150" s="12"/>
+      <c r="H150" s="12"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="14"/>
+    </row>
+    <row r="151" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E151" s="12"/>
+      <c r="F151" s="12"/>
+      <c r="G151" s="12"/>
+      <c r="H151" s="12"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="14"/>
+    </row>
+    <row r="152" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E152" s="12"/>
+      <c r="F152" s="12"/>
+      <c r="G152" s="12"/>
+      <c r="H152" s="12"/>
+      <c r="I152" s="13"/>
+      <c r="J152" s="14"/>
+    </row>
+    <row r="153" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
+      <c r="G153" s="12"/>
+      <c r="H153" s="12"/>
+      <c r="I153" s="13"/>
+      <c r="J153" s="14"/>
+    </row>
+    <row r="154" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E154" s="12"/>
+      <c r="F154" s="12"/>
+      <c r="G154" s="12"/>
+      <c r="H154" s="12"/>
+      <c r="I154" s="13"/>
+      <c r="J154" s="14"/>
+    </row>
+    <row r="155" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E155" s="12"/>
+      <c r="F155" s="12"/>
+      <c r="G155" s="12"/>
+      <c r="H155" s="12"/>
+      <c r="I155" s="13"/>
+      <c r="J155" s="14"/>
+    </row>
+    <row r="156" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E156" s="12"/>
+      <c r="F156" s="12"/>
+      <c r="G156" s="12"/>
+      <c r="H156" s="12"/>
+      <c r="I156" s="13"/>
+      <c r="J156" s="14"/>
+    </row>
+    <row r="157" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E157" s="12"/>
+      <c r="F157" s="12"/>
+      <c r="G157" s="12"/>
+      <c r="H157" s="12"/>
+      <c r="I157" s="13"/>
+      <c r="J157" s="14"/>
+    </row>
+    <row r="158" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E158" s="12"/>
+      <c r="F158" s="12"/>
+      <c r="G158" s="12"/>
+      <c r="H158" s="12"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="14"/>
+    </row>
+    <row r="159" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E159" s="12"/>
+      <c r="F159" s="12"/>
+      <c r="G159" s="12"/>
+      <c r="H159" s="12"/>
+      <c r="I159" s="13"/>
+      <c r="J159" s="14"/>
+    </row>
+    <row r="160" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E160" s="12"/>
+      <c r="F160" s="12"/>
+      <c r="G160" s="12"/>
+      <c r="H160" s="12"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="14"/>
+    </row>
+    <row r="161" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E161" s="12"/>
+      <c r="F161" s="12"/>
+      <c r="G161" s="12"/>
+      <c r="H161" s="12"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="14"/>
+    </row>
+    <row r="162" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
+      <c r="G162" s="12"/>
+      <c r="H162" s="12"/>
+      <c r="I162" s="13"/>
+      <c r="J162" s="14"/>
+    </row>
+    <row r="163" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E163" s="12"/>
+      <c r="F163" s="12"/>
+      <c r="G163" s="12"/>
+      <c r="H163" s="12"/>
+      <c r="I163" s="13"/>
+      <c r="J163" s="14"/>
+    </row>
+    <row r="164" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E164" s="12"/>
+      <c r="F164" s="12"/>
+      <c r="G164" s="12"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="13"/>
+      <c r="J164" s="14"/>
+    </row>
+    <row r="165" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E165" s="12"/>
+      <c r="F165" s="12"/>
+      <c r="G165" s="12"/>
+      <c r="H165" s="12"/>
+      <c r="I165" s="13"/>
+      <c r="J165" s="14"/>
+    </row>
+    <row r="166" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E166" s="12"/>
+      <c r="F166" s="12"/>
+      <c r="G166" s="12"/>
+      <c r="H166" s="12"/>
+      <c r="I166" s="13"/>
+      <c r="J166" s="14"/>
+    </row>
+    <row r="167" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E167" s="12"/>
+      <c r="F167" s="12"/>
+      <c r="G167" s="12"/>
+      <c r="H167" s="12"/>
+      <c r="I167" s="13"/>
+      <c r="J167" s="14"/>
+    </row>
+    <row r="168" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="13"/>
+      <c r="J168" s="14"/>
+    </row>
+    <row r="169" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E169" s="12"/>
+      <c r="F169" s="12"/>
+      <c r="G169" s="12"/>
+      <c r="H169" s="12"/>
+      <c r="I169" s="13"/>
+      <c r="J169" s="14"/>
+    </row>
+    <row r="170" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E170" s="12"/>
+      <c r="F170" s="12"/>
+      <c r="G170" s="12"/>
+      <c r="H170" s="12"/>
+      <c r="I170" s="13"/>
+      <c r="J170" s="14"/>
+    </row>
+    <row r="171" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E171" s="12"/>
+      <c r="F171" s="12"/>
+      <c r="G171" s="12"/>
+      <c r="H171" s="12"/>
+      <c r="I171" s="13"/>
+      <c r="J171" s="14"/>
+    </row>
+    <row r="172" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
+      <c r="G172" s="12"/>
+      <c r="H172" s="12"/>
+      <c r="I172" s="13"/>
+      <c r="J172" s="14"/>
+    </row>
+    <row r="173" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E173" s="12"/>
+      <c r="F173" s="12"/>
+      <c r="G173" s="12"/>
+      <c r="H173" s="12"/>
+      <c r="I173" s="13"/>
+      <c r="J173" s="14"/>
+    </row>
+    <row r="174" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E174" s="12"/>
+      <c r="F174" s="12"/>
+      <c r="G174" s="12"/>
+      <c r="H174" s="12"/>
+      <c r="I174" s="13"/>
+      <c r="J174" s="14"/>
+    </row>
+    <row r="175" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E175" s="12"/>
+      <c r="F175" s="12"/>
+      <c r="G175" s="12"/>
+      <c r="H175" s="12"/>
+      <c r="I175" s="13"/>
+      <c r="J175" s="14"/>
+    </row>
+    <row r="176" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E176" s="12"/>
+      <c r="F176" s="12"/>
+      <c r="G176" s="12"/>
+      <c r="H176" s="12"/>
+      <c r="I176" s="13"/>
+      <c r="J176" s="14"/>
+    </row>
+    <row r="177" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E177" s="12"/>
+      <c r="F177" s="12"/>
+      <c r="G177" s="12"/>
+      <c r="H177" s="12"/>
+      <c r="I177" s="13"/>
+      <c r="J177" s="14"/>
+    </row>
+    <row r="178" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E178" s="12"/>
+      <c r="F178" s="12"/>
+      <c r="G178" s="12"/>
+      <c r="H178" s="12"/>
+      <c r="I178" s="13"/>
+      <c r="J178" s="14"/>
+    </row>
+    <row r="179" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E179" s="12"/>
+      <c r="F179" s="12"/>
+      <c r="G179" s="12"/>
+      <c r="H179" s="12"/>
+      <c r="I179" s="13"/>
+      <c r="J179" s="14"/>
+    </row>
+    <row r="180" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
+      <c r="G180" s="12"/>
+      <c r="H180" s="12"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="14"/>
+    </row>
+    <row r="181" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E181" s="12"/>
+      <c r="F181" s="12"/>
+      <c r="G181" s="12"/>
+      <c r="H181" s="12"/>
+      <c r="I181" s="13"/>
+      <c r="J181" s="14"/>
+    </row>
+    <row r="182" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E182" s="12"/>
+      <c r="F182" s="12"/>
+      <c r="G182" s="12"/>
+      <c r="H182" s="12"/>
+      <c r="I182" s="13"/>
+      <c r="J182" s="14"/>
+    </row>
+    <row r="183" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E183" s="12"/>
+      <c r="F183" s="12"/>
+      <c r="G183" s="12"/>
+      <c r="H183" s="12"/>
+      <c r="I183" s="13"/>
+      <c r="J183" s="14"/>
+    </row>
+    <row r="184" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E184" s="12"/>
+      <c r="F184" s="12"/>
+      <c r="G184" s="12"/>
+      <c r="H184" s="12"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="14"/>
+    </row>
+    <row r="185" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E185" s="12"/>
+      <c r="F185" s="12"/>
+      <c r="G185" s="12"/>
+      <c r="H185" s="12"/>
+      <c r="I185" s="13"/>
+      <c r="J185" s="14"/>
+    </row>
+    <row r="186" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E186" s="12"/>
+      <c r="F186" s="12"/>
+      <c r="G186" s="12"/>
+      <c r="H186" s="12"/>
+      <c r="I186" s="13"/>
+      <c r="J186" s="14"/>
+    </row>
+    <row r="187" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E187" s="12"/>
+      <c r="F187" s="12"/>
+      <c r="G187" s="12"/>
+      <c r="H187" s="12"/>
+      <c r="I187" s="13"/>
+      <c r="J187" s="14"/>
+    </row>
+    <row r="188" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E188" s="12"/>
+      <c r="F188" s="12"/>
+      <c r="G188" s="12"/>
+      <c r="H188" s="12"/>
+      <c r="I188" s="13"/>
+      <c r="J188" s="14"/>
+    </row>
+    <row r="189" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E189" s="12"/>
+      <c r="F189" s="12"/>
+      <c r="G189" s="12"/>
+      <c r="H189" s="12"/>
+      <c r="I189" s="13"/>
+      <c r="J189" s="14"/>
+    </row>
+    <row r="190" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E190" s="12"/>
+      <c r="F190" s="12"/>
+      <c r="G190" s="12"/>
+      <c r="H190" s="12"/>
+      <c r="I190" s="13"/>
+      <c r="J190" s="14"/>
+    </row>
+    <row r="191" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E191" s="12"/>
+      <c r="F191" s="12"/>
+      <c r="G191" s="12"/>
+      <c r="H191" s="12"/>
+      <c r="I191" s="13"/>
+      <c r="J191" s="14"/>
+    </row>
+    <row r="192" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E192" s="12"/>
+      <c r="F192" s="12"/>
+      <c r="G192" s="12"/>
+      <c r="H192" s="12"/>
+      <c r="I192" s="13"/>
+      <c r="J192" s="14"/>
+    </row>
+    <row r="193" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E193" s="12"/>
+      <c r="F193" s="12"/>
+      <c r="G193" s="12"/>
+      <c r="H193" s="12"/>
+      <c r="I193" s="13"/>
+      <c r="J193" s="14"/>
+    </row>
+    <row r="194" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E194" s="12"/>
+      <c r="F194" s="12"/>
+      <c r="G194" s="12"/>
+      <c r="H194" s="12"/>
+      <c r="I194" s="13"/>
+      <c r="J194" s="14"/>
+    </row>
+    <row r="195" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E195" s="12"/>
+      <c r="F195" s="12"/>
+      <c r="G195" s="12"/>
+      <c r="H195" s="12"/>
+      <c r="I195" s="13"/>
+      <c r="J195" s="14"/>
+    </row>
+    <row r="196" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E196" s="12"/>
+      <c r="F196" s="12"/>
+      <c r="G196" s="12"/>
+      <c r="H196" s="12"/>
+      <c r="I196" s="13"/>
+      <c r="J196" s="14"/>
+    </row>
+    <row r="197" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E197" s="12"/>
+      <c r="F197" s="12"/>
+      <c r="G197" s="12"/>
+      <c r="H197" s="12"/>
+      <c r="I197" s="13"/>
+      <c r="J197" s="14"/>
+    </row>
+    <row r="198" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
+      <c r="G198" s="12"/>
+      <c r="H198" s="12"/>
+      <c r="I198" s="13"/>
+      <c r="J198" s="14"/>
+    </row>
+    <row r="199" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E199" s="12"/>
+      <c r="F199" s="12"/>
+      <c r="G199" s="12"/>
+      <c r="H199" s="12"/>
+      <c r="I199" s="13"/>
+      <c r="J199" s="14"/>
+    </row>
+    <row r="200" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E200" s="12"/>
+      <c r="F200" s="12"/>
+      <c r="G200" s="12"/>
+      <c r="H200" s="12"/>
+      <c r="I200" s="13"/>
+      <c r="J200" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Teklif aktar ve karşılaştır gridlerinde değişiklik yapıldı setup güncellendi
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
@@ -64,10 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;TL&quot;"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +127,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,10 +171,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -189,11 +194,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Yüzde" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,6 +497,7 @@
     <col min="6" max="6" width="59.26953125" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" customWidth="1"/>
     <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="13"/>
     <col min="10" max="10" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -495,7 +506,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="I1" s="12"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -503,7 +514,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-      <c r="I2" t="s">
+      <c r="I2" s="13" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="2"/>
@@ -513,7 +524,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="14"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -556,17 +567,13 @@
       <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Malzeme fiyat listesindeki excel de Para birimi sembolleri degistirildi
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/Malzeme_Fiyat_Listesi.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t>TL</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>€</t>
-  </si>
-  <si>
     <t>NAKİT</t>
   </si>
   <si>
@@ -83,11 +77,17 @@
   <si>
     <t>KART</t>
   </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;TL&quot;"/>
   </numFmts>
@@ -392,10 +392,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,27 +921,28 @@
   <dimension ref="A1:N654"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" customWidth="1"/>
-    <col min="6" max="6" width="59.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="6"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="6"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E1" s="27"/>
       <c r="F1" s="25"/>
       <c r="G1" s="4"/>
@@ -954,10 +955,10 @@
         <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E2" s="24"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -966,45 +967,45 @@
       <c r="J2" s="7"/>
       <c r="K2" s="29"/>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" ht="48.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="3"/>
       <c r="K3" s="26"/>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E4" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="28"/>
       <c r="J4" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="K4" s="32" t="s">
-        <v>17</v>
+      <c r="K4" s="31" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="F5" s="31" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1041,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1049,7 +1050,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -1058,7 +1059,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="16"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -1067,7 +1068,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -1076,7 +1077,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="16"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E11" s="13"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1085,7 +1086,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="16"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E12" s="13"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1094,7 +1095,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E13" s="13"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1103,7 +1104,7 @@
       <c r="J13" s="15"/>
       <c r="K13" s="16"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E14" s="13"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -1112,7 +1113,7 @@
       <c r="J14" s="15"/>
       <c r="K14" s="16"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1121,7 +1122,7 @@
       <c r="J15" s="15"/>
       <c r="K15" s="16"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E16" s="13"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1130,7 +1131,7 @@
       <c r="J16" s="15"/>
       <c r="K16" s="16"/>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1139,7 +1140,7 @@
       <c r="J17" s="15"/>
       <c r="K17" s="16"/>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1148,7 +1149,7 @@
       <c r="J18" s="15"/>
       <c r="K18" s="16"/>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1157,7 +1158,7 @@
       <c r="J19" s="15"/>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" s="13"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1166,7 +1167,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="16"/>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" s="13"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1175,7 +1176,7 @@
       <c r="J21" s="15"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" s="13"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1184,7 +1185,7 @@
       <c r="J22" s="15"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E23" s="13"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1193,7 +1194,7 @@
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
     </row>
-    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="13"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1202,7 +1203,7 @@
       <c r="J24" s="15"/>
       <c r="K24" s="16"/>
     </row>
-    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1211,7 +1212,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="16"/>
     </row>
-    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="13"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1220,7 +1221,7 @@
       <c r="J26" s="15"/>
       <c r="K26" s="16"/>
     </row>
-    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1229,7 +1230,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="16"/>
     </row>
-    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="13"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1238,7 +1239,7 @@
       <c r="J28" s="15"/>
       <c r="K28" s="16"/>
     </row>
-    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E29" s="13"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1247,7 +1248,7 @@
       <c r="J29" s="15"/>
       <c r="K29" s="16"/>
     </row>
-    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E30" s="13"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1256,7 +1257,7 @@
       <c r="J30" s="15"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -1265,7 +1266,7 @@
       <c r="J31" s="15"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E32" s="13"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1274,7 +1275,7 @@
       <c r="J32" s="15"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -1283,7 +1284,7 @@
       <c r="J33" s="15"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" s="13"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -1292,7 +1293,7 @@
       <c r="J34" s="15"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
@@ -1301,7 +1302,7 @@
       <c r="J35" s="15"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" s="13"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
@@ -1310,7 +1311,7 @@
       <c r="J36" s="15"/>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -1319,7 +1320,7 @@
       <c r="J37" s="15"/>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="13"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
@@ -1328,7 +1329,7 @@
       <c r="J38" s="15"/>
       <c r="K38" s="16"/>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="13"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
@@ -1337,7 +1338,7 @@
       <c r="J39" s="15"/>
       <c r="K39" s="16"/>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" s="13"/>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
@@ -1346,7 +1347,7 @@
       <c r="J40" s="15"/>
       <c r="K40" s="16"/>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" s="13"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -1355,7 +1356,7 @@
       <c r="J41" s="15"/>
       <c r="K41" s="16"/>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" s="13"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
@@ -1364,7 +1365,7 @@
       <c r="J42" s="15"/>
       <c r="K42" s="16"/>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" s="13"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -1373,7 +1374,7 @@
       <c r="J43" s="15"/>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" s="13"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
@@ -1382,7 +1383,7 @@
       <c r="J44" s="15"/>
       <c r="K44" s="16"/>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" s="13"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
@@ -1391,7 +1392,7 @@
       <c r="J45" s="15"/>
       <c r="K45" s="16"/>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" s="13"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
@@ -1400,7 +1401,7 @@
       <c r="J46" s="15"/>
       <c r="K46" s="16"/>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" s="13"/>
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
@@ -1409,7 +1410,7 @@
       <c r="J47" s="15"/>
       <c r="K47" s="16"/>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" s="13"/>
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
@@ -1418,7 +1419,7 @@
       <c r="J48" s="15"/>
       <c r="K48" s="16"/>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" s="13"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
@@ -1427,7 +1428,7 @@
       <c r="J49" s="15"/>
       <c r="K49" s="16"/>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" s="13"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
@@ -1436,7 +1437,7 @@
       <c r="J50" s="15"/>
       <c r="K50" s="16"/>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E51" s="13"/>
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
@@ -1445,7 +1446,7 @@
       <c r="J51" s="15"/>
       <c r="K51" s="16"/>
     </row>
-    <row r="52" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E52" s="13"/>
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
@@ -1454,7 +1455,7 @@
       <c r="J52" s="15"/>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E53" s="13"/>
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
@@ -1463,7 +1464,7 @@
       <c r="J53" s="15"/>
       <c r="K53" s="16"/>
     </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E54" s="13"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
@@ -1472,7 +1473,7 @@
       <c r="J54" s="15"/>
       <c r="K54" s="16"/>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E55" s="13"/>
       <c r="F55" s="14"/>
       <c r="G55" s="14"/>
@@ -1481,7 +1482,7 @@
       <c r="J55" s="15"/>
       <c r="K55" s="16"/>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E56" s="13"/>
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
@@ -1490,7 +1491,7 @@
       <c r="J56" s="15"/>
       <c r="K56" s="16"/>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E57" s="13"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
@@ -1499,7 +1500,7 @@
       <c r="J57" s="15"/>
       <c r="K57" s="16"/>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E58" s="13"/>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
@@ -1508,7 +1509,7 @@
       <c r="J58" s="15"/>
       <c r="K58" s="16"/>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E59" s="13"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
@@ -1517,7 +1518,7 @@
       <c r="J59" s="15"/>
       <c r="K59" s="16"/>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E60" s="13"/>
       <c r="F60" s="14"/>
       <c r="G60" s="14"/>
@@ -1526,7 +1527,7 @@
       <c r="J60" s="15"/>
       <c r="K60" s="16"/>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E61" s="13"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
@@ -1535,7 +1536,7 @@
       <c r="J61" s="15"/>
       <c r="K61" s="16"/>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E62" s="13"/>
       <c r="F62" s="14"/>
       <c r="G62" s="14"/>
@@ -1544,7 +1545,7 @@
       <c r="J62" s="15"/>
       <c r="K62" s="16"/>
     </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E63" s="13"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
@@ -1553,7 +1554,7 @@
       <c r="J63" s="15"/>
       <c r="K63" s="16"/>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E64" s="13"/>
       <c r="F64" s="14"/>
       <c r="G64" s="14"/>
@@ -1562,7 +1563,7 @@
       <c r="J64" s="15"/>
       <c r="K64" s="16"/>
     </row>
-    <row r="65" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E65" s="13"/>
       <c r="F65" s="14"/>
       <c r="G65" s="14"/>
@@ -1571,7 +1572,7 @@
       <c r="J65" s="15"/>
       <c r="K65" s="16"/>
     </row>
-    <row r="66" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E66" s="13"/>
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
@@ -1580,7 +1581,7 @@
       <c r="J66" s="15"/>
       <c r="K66" s="16"/>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E67" s="13"/>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
@@ -1589,7 +1590,7 @@
       <c r="J67" s="15"/>
       <c r="K67" s="16"/>
     </row>
-    <row r="68" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E68" s="13"/>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
@@ -1598,7 +1599,7 @@
       <c r="J68" s="15"/>
       <c r="K68" s="16"/>
     </row>
-    <row r="69" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E69" s="13"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
@@ -1607,7 +1608,7 @@
       <c r="J69" s="15"/>
       <c r="K69" s="16"/>
     </row>
-    <row r="70" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E70" s="13"/>
       <c r="F70" s="14"/>
       <c r="G70" s="14"/>
@@ -1616,7 +1617,7 @@
       <c r="J70" s="15"/>
       <c r="K70" s="16"/>
     </row>
-    <row r="71" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E71" s="13"/>
       <c r="F71" s="14"/>
       <c r="G71" s="14"/>
@@ -1625,7 +1626,7 @@
       <c r="J71" s="15"/>
       <c r="K71" s="16"/>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E72" s="13"/>
       <c r="F72" s="14"/>
       <c r="G72" s="14"/>
@@ -1634,7 +1635,7 @@
       <c r="J72" s="15"/>
       <c r="K72" s="16"/>
     </row>
-    <row r="73" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E73" s="13"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
@@ -1643,7 +1644,7 @@
       <c r="J73" s="15"/>
       <c r="K73" s="16"/>
     </row>
-    <row r="74" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E74" s="13"/>
       <c r="F74" s="14"/>
       <c r="G74" s="14"/>
@@ -1652,7 +1653,7 @@
       <c r="J74" s="15"/>
       <c r="K74" s="16"/>
     </row>
-    <row r="75" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E75" s="13"/>
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
@@ -1661,7 +1662,7 @@
       <c r="J75" s="15"/>
       <c r="K75" s="16"/>
     </row>
-    <row r="76" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E76" s="13"/>
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
@@ -1670,7 +1671,7 @@
       <c r="J76" s="15"/>
       <c r="K76" s="16"/>
     </row>
-    <row r="77" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E77" s="13"/>
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
@@ -1679,7 +1680,7 @@
       <c r="J77" s="15"/>
       <c r="K77" s="16"/>
     </row>
-    <row r="78" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E78" s="13"/>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
@@ -1688,7 +1689,7 @@
       <c r="J78" s="15"/>
       <c r="K78" s="16"/>
     </row>
-    <row r="79" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E79" s="13"/>
       <c r="F79" s="14"/>
       <c r="G79" s="14"/>
@@ -1697,7 +1698,7 @@
       <c r="J79" s="15"/>
       <c r="K79" s="16"/>
     </row>
-    <row r="80" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E80" s="13"/>
       <c r="F80" s="14"/>
       <c r="G80" s="14"/>
@@ -1706,7 +1707,7 @@
       <c r="J80" s="15"/>
       <c r="K80" s="16"/>
     </row>
-    <row r="81" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E81" s="13"/>
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
@@ -1715,7 +1716,7 @@
       <c r="J81" s="15"/>
       <c r="K81" s="16"/>
     </row>
-    <row r="82" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E82" s="13"/>
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
@@ -1724,7 +1725,7 @@
       <c r="J82" s="15"/>
       <c r="K82" s="16"/>
     </row>
-    <row r="83" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E83" s="13"/>
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
@@ -1733,7 +1734,7 @@
       <c r="J83" s="15"/>
       <c r="K83" s="16"/>
     </row>
-    <row r="84" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E84" s="13"/>
       <c r="F84" s="14"/>
       <c r="G84" s="14"/>
@@ -1742,7 +1743,7 @@
       <c r="J84" s="15"/>
       <c r="K84" s="16"/>
     </row>
-    <row r="85" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E85" s="13"/>
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
@@ -1751,7 +1752,7 @@
       <c r="J85" s="15"/>
       <c r="K85" s="16"/>
     </row>
-    <row r="86" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E86" s="13"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
@@ -1760,7 +1761,7 @@
       <c r="J86" s="15"/>
       <c r="K86" s="16"/>
     </row>
-    <row r="87" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E87" s="13"/>
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
@@ -1769,7 +1770,7 @@
       <c r="J87" s="15"/>
       <c r="K87" s="16"/>
     </row>
-    <row r="88" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E88" s="13"/>
       <c r="F88" s="14"/>
       <c r="G88" s="14"/>
@@ -1778,7 +1779,7 @@
       <c r="J88" s="15"/>
       <c r="K88" s="16"/>
     </row>
-    <row r="89" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E89" s="13"/>
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
@@ -1787,7 +1788,7 @@
       <c r="J89" s="15"/>
       <c r="K89" s="16"/>
     </row>
-    <row r="90" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E90" s="13"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
@@ -1796,7 +1797,7 @@
       <c r="J90" s="15"/>
       <c r="K90" s="16"/>
     </row>
-    <row r="91" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E91" s="13"/>
       <c r="F91" s="14"/>
       <c r="G91" s="14"/>
@@ -1805,7 +1806,7 @@
       <c r="J91" s="15"/>
       <c r="K91" s="16"/>
     </row>
-    <row r="92" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E92" s="13"/>
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
@@ -1814,7 +1815,7 @@
       <c r="J92" s="15"/>
       <c r="K92" s="16"/>
     </row>
-    <row r="93" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E93" s="13"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
@@ -1823,7 +1824,7 @@
       <c r="J93" s="15"/>
       <c r="K93" s="16"/>
     </row>
-    <row r="94" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E94" s="13"/>
       <c r="F94" s="14"/>
       <c r="G94" s="14"/>
@@ -1832,7 +1833,7 @@
       <c r="J94" s="15"/>
       <c r="K94" s="16"/>
     </row>
-    <row r="95" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E95" s="13"/>
       <c r="F95" s="14"/>
       <c r="G95" s="14"/>
@@ -1841,7 +1842,7 @@
       <c r="J95" s="15"/>
       <c r="K95" s="16"/>
     </row>
-    <row r="96" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E96" s="13"/>
       <c r="F96" s="14"/>
       <c r="G96" s="14"/>
@@ -1850,7 +1851,7 @@
       <c r="J96" s="15"/>
       <c r="K96" s="16"/>
     </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E97" s="13"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
@@ -1859,7 +1860,7 @@
       <c r="J97" s="15"/>
       <c r="K97" s="16"/>
     </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E98" s="13"/>
       <c r="F98" s="14"/>
       <c r="G98" s="14"/>
@@ -1868,7 +1869,7 @@
       <c r="J98" s="15"/>
       <c r="K98" s="16"/>
     </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E99" s="13"/>
       <c r="F99" s="14"/>
       <c r="G99" s="14"/>
@@ -1877,7 +1878,7 @@
       <c r="J99" s="15"/>
       <c r="K99" s="16"/>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E100" s="13"/>
       <c r="F100" s="14"/>
       <c r="G100" s="14"/>
@@ -1886,7 +1887,7 @@
       <c r="J100" s="15"/>
       <c r="K100" s="16"/>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E101" s="13"/>
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
@@ -1895,7 +1896,7 @@
       <c r="J101" s="15"/>
       <c r="K101" s="16"/>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E102" s="13"/>
       <c r="F102" s="14"/>
       <c r="G102" s="14"/>
@@ -1904,7 +1905,7 @@
       <c r="J102" s="15"/>
       <c r="K102" s="16"/>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E103" s="13"/>
       <c r="F103" s="14"/>
       <c r="G103" s="14"/>
@@ -1913,7 +1914,7 @@
       <c r="J103" s="15"/>
       <c r="K103" s="16"/>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E104" s="13"/>
       <c r="F104" s="14"/>
       <c r="G104" s="14"/>
@@ -1922,7 +1923,7 @@
       <c r="J104" s="15"/>
       <c r="K104" s="16"/>
     </row>
-    <row r="105" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E105" s="13"/>
       <c r="F105" s="14"/>
       <c r="G105" s="14"/>
@@ -1931,7 +1932,7 @@
       <c r="J105" s="15"/>
       <c r="K105" s="16"/>
     </row>
-    <row r="106" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E106" s="13"/>
       <c r="F106" s="14"/>
       <c r="G106" s="14"/>
@@ -1940,7 +1941,7 @@
       <c r="J106" s="15"/>
       <c r="K106" s="16"/>
     </row>
-    <row r="107" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E107" s="13"/>
       <c r="F107" s="14"/>
       <c r="G107" s="14"/>
@@ -1949,7 +1950,7 @@
       <c r="J107" s="15"/>
       <c r="K107" s="16"/>
     </row>
-    <row r="108" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E108" s="13"/>
       <c r="F108" s="14"/>
       <c r="G108" s="14"/>
@@ -1958,7 +1959,7 @@
       <c r="J108" s="15"/>
       <c r="K108" s="16"/>
     </row>
-    <row r="109" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E109" s="13"/>
       <c r="F109" s="14"/>
       <c r="G109" s="14"/>
@@ -1967,7 +1968,7 @@
       <c r="J109" s="15"/>
       <c r="K109" s="16"/>
     </row>
-    <row r="110" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E110" s="13"/>
       <c r="F110" s="14"/>
       <c r="G110" s="14"/>
@@ -1976,7 +1977,7 @@
       <c r="J110" s="15"/>
       <c r="K110" s="16"/>
     </row>
-    <row r="111" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E111" s="13"/>
       <c r="F111" s="14"/>
       <c r="G111" s="14"/>
@@ -1985,7 +1986,7 @@
       <c r="J111" s="15"/>
       <c r="K111" s="16"/>
     </row>
-    <row r="112" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E112" s="13"/>
       <c r="F112" s="14"/>
       <c r="G112" s="14"/>
@@ -1994,7 +1995,7 @@
       <c r="J112" s="15"/>
       <c r="K112" s="16"/>
     </row>
-    <row r="113" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E113" s="13"/>
       <c r="F113" s="14"/>
       <c r="G113" s="14"/>
@@ -2003,7 +2004,7 @@
       <c r="J113" s="15"/>
       <c r="K113" s="16"/>
     </row>
-    <row r="114" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E114" s="13"/>
       <c r="F114" s="14"/>
       <c r="G114" s="14"/>
@@ -2012,7 +2013,7 @@
       <c r="J114" s="15"/>
       <c r="K114" s="16"/>
     </row>
-    <row r="115" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E115" s="13"/>
       <c r="F115" s="14"/>
       <c r="G115" s="14"/>
@@ -2021,7 +2022,7 @@
       <c r="J115" s="15"/>
       <c r="K115" s="16"/>
     </row>
-    <row r="116" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E116" s="13"/>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -2030,7 +2031,7 @@
       <c r="J116" s="15"/>
       <c r="K116" s="16"/>
     </row>
-    <row r="117" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E117" s="13"/>
       <c r="F117" s="14"/>
       <c r="G117" s="14"/>
@@ -2039,7 +2040,7 @@
       <c r="J117" s="15"/>
       <c r="K117" s="16"/>
     </row>
-    <row r="118" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E118" s="13"/>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
@@ -2048,7 +2049,7 @@
       <c r="J118" s="15"/>
       <c r="K118" s="16"/>
     </row>
-    <row r="119" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E119" s="13"/>
       <c r="F119" s="14"/>
       <c r="G119" s="14"/>
@@ -2057,7 +2058,7 @@
       <c r="J119" s="15"/>
       <c r="K119" s="16"/>
     </row>
-    <row r="120" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E120" s="13"/>
       <c r="F120" s="14"/>
       <c r="G120" s="14"/>
@@ -2066,7 +2067,7 @@
       <c r="J120" s="15"/>
       <c r="K120" s="16"/>
     </row>
-    <row r="121" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E121" s="13"/>
       <c r="F121" s="14"/>
       <c r="G121" s="14"/>
@@ -2075,7 +2076,7 @@
       <c r="J121" s="15"/>
       <c r="K121" s="16"/>
     </row>
-    <row r="122" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E122" s="13"/>
       <c r="F122" s="14"/>
       <c r="G122" s="14"/>
@@ -2084,7 +2085,7 @@
       <c r="J122" s="15"/>
       <c r="K122" s="16"/>
     </row>
-    <row r="123" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E123" s="13"/>
       <c r="F123" s="14"/>
       <c r="G123" s="14"/>
@@ -2093,7 +2094,7 @@
       <c r="J123" s="15"/>
       <c r="K123" s="16"/>
     </row>
-    <row r="124" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E124" s="13"/>
       <c r="F124" s="14"/>
       <c r="G124" s="14"/>
@@ -2102,7 +2103,7 @@
       <c r="J124" s="15"/>
       <c r="K124" s="16"/>
     </row>
-    <row r="125" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E125" s="13"/>
       <c r="F125" s="14"/>
       <c r="G125" s="14"/>
@@ -2111,7 +2112,7 @@
       <c r="J125" s="15"/>
       <c r="K125" s="16"/>
     </row>
-    <row r="126" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E126" s="13"/>
       <c r="F126" s="14"/>
       <c r="G126" s="14"/>
@@ -2120,7 +2121,7 @@
       <c r="J126" s="15"/>
       <c r="K126" s="16"/>
     </row>
-    <row r="127" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E127" s="13"/>
       <c r="F127" s="14"/>
       <c r="G127" s="14"/>
@@ -2129,7 +2130,7 @@
       <c r="J127" s="15"/>
       <c r="K127" s="16"/>
     </row>
-    <row r="128" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E128" s="13"/>
       <c r="F128" s="14"/>
       <c r="G128" s="14"/>
@@ -2138,7 +2139,7 @@
       <c r="J128" s="15"/>
       <c r="K128" s="16"/>
     </row>
-    <row r="129" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E129" s="13"/>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -2147,7 +2148,7 @@
       <c r="J129" s="15"/>
       <c r="K129" s="16"/>
     </row>
-    <row r="130" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E130" s="13"/>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -2156,7 +2157,7 @@
       <c r="J130" s="15"/>
       <c r="K130" s="16"/>
     </row>
-    <row r="131" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E131" s="13"/>
       <c r="F131" s="14"/>
       <c r="G131" s="14"/>
@@ -2165,7 +2166,7 @@
       <c r="J131" s="15"/>
       <c r="K131" s="16"/>
     </row>
-    <row r="132" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E132" s="13"/>
       <c r="F132" s="14"/>
       <c r="G132" s="14"/>
@@ -2174,7 +2175,7 @@
       <c r="J132" s="15"/>
       <c r="K132" s="16"/>
     </row>
-    <row r="133" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E133" s="13"/>
       <c r="F133" s="14"/>
       <c r="G133" s="14"/>
@@ -2183,7 +2184,7 @@
       <c r="J133" s="15"/>
       <c r="K133" s="16"/>
     </row>
-    <row r="134" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E134" s="13"/>
       <c r="F134" s="14"/>
       <c r="G134" s="14"/>
@@ -2192,7 +2193,7 @@
       <c r="J134" s="15"/>
       <c r="K134" s="16"/>
     </row>
-    <row r="135" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E135" s="13"/>
       <c r="F135" s="14"/>
       <c r="G135" s="14"/>
@@ -2201,7 +2202,7 @@
       <c r="J135" s="15"/>
       <c r="K135" s="16"/>
     </row>
-    <row r="136" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E136" s="13"/>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -2210,7 +2211,7 @@
       <c r="J136" s="15"/>
       <c r="K136" s="16"/>
     </row>
-    <row r="137" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E137" s="13"/>
       <c r="F137" s="14"/>
       <c r="G137" s="14"/>
@@ -2219,7 +2220,7 @@
       <c r="J137" s="15"/>
       <c r="K137" s="16"/>
     </row>
-    <row r="138" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E138" s="13"/>
       <c r="F138" s="14"/>
       <c r="G138" s="14"/>
@@ -2228,7 +2229,7 @@
       <c r="J138" s="15"/>
       <c r="K138" s="16"/>
     </row>
-    <row r="139" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="139" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E139" s="13"/>
       <c r="F139" s="14"/>
       <c r="G139" s="14"/>
@@ -2237,7 +2238,7 @@
       <c r="J139" s="15"/>
       <c r="K139" s="16"/>
     </row>
-    <row r="140" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="140" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E140" s="13"/>
       <c r="F140" s="14"/>
       <c r="G140" s="14"/>
@@ -2246,7 +2247,7 @@
       <c r="J140" s="15"/>
       <c r="K140" s="16"/>
     </row>
-    <row r="141" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="141" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E141" s="13"/>
       <c r="F141" s="14"/>
       <c r="G141" s="14"/>
@@ -2255,7 +2256,7 @@
       <c r="J141" s="15"/>
       <c r="K141" s="16"/>
     </row>
-    <row r="142" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E142" s="13"/>
       <c r="F142" s="14"/>
       <c r="G142" s="14"/>
@@ -2264,7 +2265,7 @@
       <c r="J142" s="15"/>
       <c r="K142" s="16"/>
     </row>
-    <row r="143" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E143" s="13"/>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -2273,7 +2274,7 @@
       <c r="J143" s="15"/>
       <c r="K143" s="16"/>
     </row>
-    <row r="144" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E144" s="13"/>
       <c r="F144" s="14"/>
       <c r="G144" s="14"/>
@@ -2282,7 +2283,7 @@
       <c r="J144" s="15"/>
       <c r="K144" s="16"/>
     </row>
-    <row r="145" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E145" s="13"/>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
@@ -2291,7 +2292,7 @@
       <c r="J145" s="15"/>
       <c r="K145" s="16"/>
     </row>
-    <row r="146" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E146" s="13"/>
       <c r="F146" s="14"/>
       <c r="G146" s="14"/>
@@ -2300,7 +2301,7 @@
       <c r="J146" s="15"/>
       <c r="K146" s="16"/>
     </row>
-    <row r="147" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E147" s="13"/>
       <c r="F147" s="14"/>
       <c r="G147" s="14"/>
@@ -2309,7 +2310,7 @@
       <c r="J147" s="15"/>
       <c r="K147" s="16"/>
     </row>
-    <row r="148" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E148" s="13"/>
       <c r="F148" s="14"/>
       <c r="G148" s="14"/>
@@ -2318,7 +2319,7 @@
       <c r="J148" s="15"/>
       <c r="K148" s="16"/>
     </row>
-    <row r="149" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E149" s="13"/>
       <c r="F149" s="14"/>
       <c r="G149" s="14"/>
@@ -2327,7 +2328,7 @@
       <c r="J149" s="15"/>
       <c r="K149" s="16"/>
     </row>
-    <row r="150" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="150" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E150" s="13"/>
       <c r="F150" s="14"/>
       <c r="G150" s="14"/>
@@ -2336,7 +2337,7 @@
       <c r="J150" s="15"/>
       <c r="K150" s="16"/>
     </row>
-    <row r="151" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E151" s="13"/>
       <c r="F151" s="14"/>
       <c r="G151" s="14"/>
@@ -2345,7 +2346,7 @@
       <c r="J151" s="15"/>
       <c r="K151" s="16"/>
     </row>
-    <row r="152" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E152" s="13"/>
       <c r="F152" s="14"/>
       <c r="G152" s="14"/>
@@ -2354,7 +2355,7 @@
       <c r="J152" s="15"/>
       <c r="K152" s="16"/>
     </row>
-    <row r="153" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="153" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E153" s="13"/>
       <c r="F153" s="14"/>
       <c r="G153" s="14"/>
@@ -2363,7 +2364,7 @@
       <c r="J153" s="15"/>
       <c r="K153" s="16"/>
     </row>
-    <row r="154" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E154" s="13"/>
       <c r="F154" s="14"/>
       <c r="G154" s="14"/>
@@ -2372,7 +2373,7 @@
       <c r="J154" s="15"/>
       <c r="K154" s="16"/>
     </row>
-    <row r="155" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E155" s="13"/>
       <c r="F155" s="14"/>
       <c r="G155" s="14"/>
@@ -2381,7 +2382,7 @@
       <c r="J155" s="15"/>
       <c r="K155" s="16"/>
     </row>
-    <row r="156" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E156" s="13"/>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -2390,7 +2391,7 @@
       <c r="J156" s="15"/>
       <c r="K156" s="16"/>
     </row>
-    <row r="157" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="157" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E157" s="13"/>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -2399,7 +2400,7 @@
       <c r="J157" s="15"/>
       <c r="K157" s="16"/>
     </row>
-    <row r="158" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E158" s="13"/>
       <c r="F158" s="14"/>
       <c r="G158" s="14"/>
@@ -2408,7 +2409,7 @@
       <c r="J158" s="15"/>
       <c r="K158" s="16"/>
     </row>
-    <row r="159" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E159" s="13"/>
       <c r="F159" s="14"/>
       <c r="G159" s="14"/>
@@ -2417,7 +2418,7 @@
       <c r="J159" s="15"/>
       <c r="K159" s="16"/>
     </row>
-    <row r="160" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E160" s="13"/>
       <c r="F160" s="14"/>
       <c r="G160" s="14"/>
@@ -2426,7 +2427,7 @@
       <c r="J160" s="15"/>
       <c r="K160" s="16"/>
     </row>
-    <row r="161" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="161" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E161" s="13"/>
       <c r="F161" s="14"/>
       <c r="G161" s="14"/>
@@ -2435,7 +2436,7 @@
       <c r="J161" s="15"/>
       <c r="K161" s="16"/>
     </row>
-    <row r="162" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="162" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E162" s="13"/>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
@@ -2444,7 +2445,7 @@
       <c r="J162" s="15"/>
       <c r="K162" s="16"/>
     </row>
-    <row r="163" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="163" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E163" s="13"/>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -2453,7 +2454,7 @@
       <c r="J163" s="15"/>
       <c r="K163" s="16"/>
     </row>
-    <row r="164" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="164" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E164" s="13"/>
       <c r="F164" s="14"/>
       <c r="G164" s="14"/>
@@ -2462,7 +2463,7 @@
       <c r="J164" s="15"/>
       <c r="K164" s="16"/>
     </row>
-    <row r="165" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="165" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E165" s="13"/>
       <c r="F165" s="14"/>
       <c r="G165" s="14"/>
@@ -2471,7 +2472,7 @@
       <c r="J165" s="15"/>
       <c r="K165" s="16"/>
     </row>
-    <row r="166" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="166" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E166" s="13"/>
       <c r="F166" s="14"/>
       <c r="G166" s="14"/>
@@ -2480,7 +2481,7 @@
       <c r="J166" s="15"/>
       <c r="K166" s="16"/>
     </row>
-    <row r="167" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="167" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E167" s="13"/>
       <c r="F167" s="14"/>
       <c r="G167" s="14"/>
@@ -2489,7 +2490,7 @@
       <c r="J167" s="15"/>
       <c r="K167" s="16"/>
     </row>
-    <row r="168" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="168" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E168" s="13"/>
       <c r="F168" s="14"/>
       <c r="G168" s="14"/>
@@ -2498,7 +2499,7 @@
       <c r="J168" s="15"/>
       <c r="K168" s="16"/>
     </row>
-    <row r="169" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="169" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E169" s="13"/>
       <c r="F169" s="14"/>
       <c r="G169" s="14"/>
@@ -2507,7 +2508,7 @@
       <c r="J169" s="15"/>
       <c r="K169" s="16"/>
     </row>
-    <row r="170" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="170" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E170" s="13"/>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -2516,7 +2517,7 @@
       <c r="J170" s="15"/>
       <c r="K170" s="16"/>
     </row>
-    <row r="171" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="171" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E171" s="13"/>
       <c r="F171" s="14"/>
       <c r="G171" s="14"/>
@@ -2525,7 +2526,7 @@
       <c r="J171" s="15"/>
       <c r="K171" s="16"/>
     </row>
-    <row r="172" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="172" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E172" s="13"/>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -2534,7 +2535,7 @@
       <c r="J172" s="15"/>
       <c r="K172" s="16"/>
     </row>
-    <row r="173" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="173" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E173" s="13"/>
       <c r="F173" s="14"/>
       <c r="G173" s="14"/>
@@ -2543,7 +2544,7 @@
       <c r="J173" s="15"/>
       <c r="K173" s="16"/>
     </row>
-    <row r="174" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="174" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E174" s="13"/>
       <c r="F174" s="14"/>
       <c r="G174" s="14"/>
@@ -2552,7 +2553,7 @@
       <c r="J174" s="15"/>
       <c r="K174" s="16"/>
     </row>
-    <row r="175" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="175" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E175" s="13"/>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -2561,7 +2562,7 @@
       <c r="J175" s="15"/>
       <c r="K175" s="16"/>
     </row>
-    <row r="176" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="176" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E176" s="13"/>
       <c r="F176" s="14"/>
       <c r="G176" s="14"/>
@@ -2570,7 +2571,7 @@
       <c r="J176" s="15"/>
       <c r="K176" s="16"/>
     </row>
-    <row r="177" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="177" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E177" s="13"/>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
@@ -2579,7 +2580,7 @@
       <c r="J177" s="15"/>
       <c r="K177" s="16"/>
     </row>
-    <row r="178" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="178" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E178" s="13"/>
       <c r="F178" s="14"/>
       <c r="G178" s="14"/>
@@ -2588,7 +2589,7 @@
       <c r="J178" s="15"/>
       <c r="K178" s="16"/>
     </row>
-    <row r="179" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="179" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E179" s="13"/>
       <c r="F179" s="14"/>
       <c r="G179" s="14"/>
@@ -2597,7 +2598,7 @@
       <c r="J179" s="15"/>
       <c r="K179" s="16"/>
     </row>
-    <row r="180" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="180" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E180" s="13"/>
       <c r="F180" s="14"/>
       <c r="G180" s="14"/>
@@ -2606,7 +2607,7 @@
       <c r="J180" s="15"/>
       <c r="K180" s="16"/>
     </row>
-    <row r="181" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="181" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E181" s="13"/>
       <c r="F181" s="14"/>
       <c r="G181" s="14"/>
@@ -2615,7 +2616,7 @@
       <c r="J181" s="15"/>
       <c r="K181" s="16"/>
     </row>
-    <row r="182" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="182" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E182" s="13"/>
       <c r="F182" s="14"/>
       <c r="G182" s="14"/>
@@ -2624,7 +2625,7 @@
       <c r="J182" s="15"/>
       <c r="K182" s="16"/>
     </row>
-    <row r="183" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="183" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E183" s="13"/>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -2633,7 +2634,7 @@
       <c r="J183" s="15"/>
       <c r="K183" s="16"/>
     </row>
-    <row r="184" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="184" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E184" s="13"/>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -2642,7 +2643,7 @@
       <c r="J184" s="15"/>
       <c r="K184" s="16"/>
     </row>
-    <row r="185" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="185" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E185" s="13"/>
       <c r="F185" s="14"/>
       <c r="G185" s="14"/>
@@ -2651,7 +2652,7 @@
       <c r="J185" s="15"/>
       <c r="K185" s="16"/>
     </row>
-    <row r="186" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="186" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E186" s="13"/>
       <c r="F186" s="14"/>
       <c r="G186" s="14"/>
@@ -2660,7 +2661,7 @@
       <c r="J186" s="15"/>
       <c r="K186" s="16"/>
     </row>
-    <row r="187" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="187" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E187" s="13"/>
       <c r="F187" s="14"/>
       <c r="G187" s="14"/>
@@ -2669,7 +2670,7 @@
       <c r="J187" s="15"/>
       <c r="K187" s="16"/>
     </row>
-    <row r="188" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="188" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E188" s="13"/>
       <c r="F188" s="14"/>
       <c r="G188" s="14"/>
@@ -2678,7 +2679,7 @@
       <c r="J188" s="15"/>
       <c r="K188" s="16"/>
     </row>
-    <row r="189" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="189" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E189" s="13"/>
       <c r="F189" s="14"/>
       <c r="G189" s="14"/>
@@ -2687,7 +2688,7 @@
       <c r="J189" s="15"/>
       <c r="K189" s="16"/>
     </row>
-    <row r="190" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="190" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E190" s="13"/>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -2696,7 +2697,7 @@
       <c r="J190" s="15"/>
       <c r="K190" s="16"/>
     </row>
-    <row r="191" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="191" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E191" s="13"/>
       <c r="F191" s="14"/>
       <c r="G191" s="14"/>
@@ -2705,7 +2706,7 @@
       <c r="J191" s="15"/>
       <c r="K191" s="16"/>
     </row>
-    <row r="192" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="192" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E192" s="13"/>
       <c r="F192" s="14"/>
       <c r="G192" s="14"/>
@@ -2714,7 +2715,7 @@
       <c r="J192" s="15"/>
       <c r="K192" s="16"/>
     </row>
-    <row r="193" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="193" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E193" s="13"/>
       <c r="F193" s="14"/>
       <c r="G193" s="14"/>
@@ -2723,7 +2724,7 @@
       <c r="J193" s="15"/>
       <c r="K193" s="16"/>
     </row>
-    <row r="194" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="194" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E194" s="13"/>
       <c r="F194" s="14"/>
       <c r="G194" s="14"/>
@@ -2732,7 +2733,7 @@
       <c r="J194" s="15"/>
       <c r="K194" s="16"/>
     </row>
-    <row r="195" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="195" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E195" s="13"/>
       <c r="F195" s="14"/>
       <c r="G195" s="14"/>
@@ -2741,7 +2742,7 @@
       <c r="J195" s="15"/>
       <c r="K195" s="16"/>
     </row>
-    <row r="196" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="196" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E196" s="13"/>
       <c r="F196" s="14"/>
       <c r="G196" s="14"/>
@@ -2750,7 +2751,7 @@
       <c r="J196" s="15"/>
       <c r="K196" s="16"/>
     </row>
-    <row r="197" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="197" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E197" s="13"/>
       <c r="F197" s="14"/>
       <c r="G197" s="14"/>
@@ -2759,7 +2760,7 @@
       <c r="J197" s="15"/>
       <c r="K197" s="16"/>
     </row>
-    <row r="198" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="198" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E198" s="13"/>
       <c r="F198" s="14"/>
       <c r="G198" s="14"/>
@@ -2768,7 +2769,7 @@
       <c r="J198" s="15"/>
       <c r="K198" s="16"/>
     </row>
-    <row r="199" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="199" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E199" s="13"/>
       <c r="F199" s="14"/>
       <c r="G199" s="14"/>
@@ -2777,7 +2778,7 @@
       <c r="J199" s="15"/>
       <c r="K199" s="16"/>
     </row>
-    <row r="200" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="200" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E200" s="13"/>
       <c r="F200" s="14"/>
       <c r="G200" s="14"/>
@@ -2786,7 +2787,7 @@
       <c r="J200" s="15"/>
       <c r="K200" s="16"/>
     </row>
-    <row r="201" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="201" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E201" s="13"/>
       <c r="F201" s="14"/>
       <c r="G201" s="14"/>
@@ -2795,7 +2796,7 @@
       <c r="J201" s="15"/>
       <c r="K201" s="16"/>
     </row>
-    <row r="202" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="202" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E202" s="13"/>
       <c r="F202" s="14"/>
       <c r="G202" s="14"/>
@@ -2804,7 +2805,7 @@
       <c r="J202" s="15"/>
       <c r="K202" s="16"/>
     </row>
-    <row r="203" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="203" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E203" s="13"/>
       <c r="F203" s="14"/>
       <c r="G203" s="14"/>
@@ -2813,7 +2814,7 @@
       <c r="J203" s="15"/>
       <c r="K203" s="16"/>
     </row>
-    <row r="204" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="204" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E204" s="13"/>
       <c r="F204" s="14"/>
       <c r="G204" s="14"/>
@@ -2822,7 +2823,7 @@
       <c r="J204" s="15"/>
       <c r="K204" s="16"/>
     </row>
-    <row r="205" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="205" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E205" s="13"/>
       <c r="F205" s="14"/>
       <c r="G205" s="14"/>
@@ -2831,7 +2832,7 @@
       <c r="J205" s="15"/>
       <c r="K205" s="16"/>
     </row>
-    <row r="206" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="206" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E206" s="13"/>
       <c r="F206" s="14"/>
       <c r="G206" s="14"/>
@@ -2840,7 +2841,7 @@
       <c r="J206" s="15"/>
       <c r="K206" s="16"/>
     </row>
-    <row r="207" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="207" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E207" s="13"/>
       <c r="F207" s="14"/>
       <c r="G207" s="14"/>
@@ -2849,7 +2850,7 @@
       <c r="J207" s="15"/>
       <c r="K207" s="16"/>
     </row>
-    <row r="208" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="208" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E208" s="13"/>
       <c r="F208" s="14"/>
       <c r="G208" s="14"/>
@@ -2858,7 +2859,7 @@
       <c r="J208" s="15"/>
       <c r="K208" s="16"/>
     </row>
-    <row r="209" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="209" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E209" s="13"/>
       <c r="F209" s="14"/>
       <c r="G209" s="14"/>
@@ -2867,7 +2868,7 @@
       <c r="J209" s="15"/>
       <c r="K209" s="16"/>
     </row>
-    <row r="210" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="210" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E210" s="13"/>
       <c r="F210" s="14"/>
       <c r="G210" s="14"/>
@@ -2876,7 +2877,7 @@
       <c r="J210" s="15"/>
       <c r="K210" s="16"/>
     </row>
-    <row r="211" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="211" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E211" s="13"/>
       <c r="F211" s="14"/>
       <c r="G211" s="14"/>
@@ -2885,7 +2886,7 @@
       <c r="J211" s="15"/>
       <c r="K211" s="16"/>
     </row>
-    <row r="212" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="212" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E212" s="13"/>
       <c r="F212" s="14"/>
       <c r="G212" s="14"/>
@@ -2894,7 +2895,7 @@
       <c r="J212" s="15"/>
       <c r="K212" s="16"/>
     </row>
-    <row r="213" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="213" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E213" s="13"/>
       <c r="F213" s="14"/>
       <c r="G213" s="14"/>
@@ -2903,7 +2904,7 @@
       <c r="J213" s="15"/>
       <c r="K213" s="16"/>
     </row>
-    <row r="214" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="214" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E214" s="13"/>
       <c r="F214" s="14"/>
       <c r="G214" s="14"/>
@@ -2912,7 +2913,7 @@
       <c r="J214" s="15"/>
       <c r="K214" s="16"/>
     </row>
-    <row r="215" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="215" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E215" s="13"/>
       <c r="F215" s="14"/>
       <c r="G215" s="14"/>
@@ -2921,7 +2922,7 @@
       <c r="J215" s="15"/>
       <c r="K215" s="16"/>
     </row>
-    <row r="216" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="216" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E216" s="13"/>
       <c r="F216" s="14"/>
       <c r="G216" s="14"/>
@@ -2930,7 +2931,7 @@
       <c r="J216" s="15"/>
       <c r="K216" s="16"/>
     </row>
-    <row r="217" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="217" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E217" s="13"/>
       <c r="F217" s="14"/>
       <c r="G217" s="14"/>
@@ -2939,7 +2940,7 @@
       <c r="J217" s="15"/>
       <c r="K217" s="16"/>
     </row>
-    <row r="218" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="218" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E218" s="13"/>
       <c r="F218" s="14"/>
       <c r="G218" s="14"/>
@@ -2948,7 +2949,7 @@
       <c r="J218" s="15"/>
       <c r="K218" s="16"/>
     </row>
-    <row r="219" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="219" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E219" s="13"/>
       <c r="F219" s="14"/>
       <c r="G219" s="14"/>
@@ -2957,7 +2958,7 @@
       <c r="J219" s="15"/>
       <c r="K219" s="16"/>
     </row>
-    <row r="220" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="220" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E220" s="13"/>
       <c r="F220" s="14"/>
       <c r="G220" s="14"/>
@@ -2966,7 +2967,7 @@
       <c r="J220" s="15"/>
       <c r="K220" s="16"/>
     </row>
-    <row r="221" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="221" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E221" s="13"/>
       <c r="F221" s="14"/>
       <c r="G221" s="14"/>
@@ -2975,7 +2976,7 @@
       <c r="J221" s="15"/>
       <c r="K221" s="16"/>
     </row>
-    <row r="222" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="222" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E222" s="13"/>
       <c r="F222" s="14"/>
       <c r="G222" s="14"/>
@@ -2984,7 +2985,7 @@
       <c r="J222" s="15"/>
       <c r="K222" s="16"/>
     </row>
-    <row r="223" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="223" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E223" s="13"/>
       <c r="F223" s="14"/>
       <c r="G223" s="14"/>
@@ -2993,7 +2994,7 @@
       <c r="J223" s="15"/>
       <c r="K223" s="16"/>
     </row>
-    <row r="224" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="224" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E224" s="13"/>
       <c r="F224" s="14"/>
       <c r="G224" s="14"/>
@@ -3002,7 +3003,7 @@
       <c r="J224" s="15"/>
       <c r="K224" s="16"/>
     </row>
-    <row r="225" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="225" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E225" s="13"/>
       <c r="F225" s="14"/>
       <c r="G225" s="14"/>
@@ -3011,7 +3012,7 @@
       <c r="J225" s="15"/>
       <c r="K225" s="16"/>
     </row>
-    <row r="226" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="226" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E226" s="13"/>
       <c r="F226" s="14"/>
       <c r="G226" s="14"/>
@@ -3020,7 +3021,7 @@
       <c r="J226" s="15"/>
       <c r="K226" s="16"/>
     </row>
-    <row r="227" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="227" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E227" s="13"/>
       <c r="F227" s="14"/>
       <c r="G227" s="14"/>
@@ -3029,7 +3030,7 @@
       <c r="J227" s="15"/>
       <c r="K227" s="16"/>
     </row>
-    <row r="228" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="228" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E228" s="13"/>
       <c r="F228" s="14"/>
       <c r="G228" s="14"/>
@@ -3038,7 +3039,7 @@
       <c r="J228" s="15"/>
       <c r="K228" s="16"/>
     </row>
-    <row r="229" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="229" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E229" s="13"/>
       <c r="F229" s="14"/>
       <c r="G229" s="14"/>
@@ -3047,7 +3048,7 @@
       <c r="J229" s="15"/>
       <c r="K229" s="16"/>
     </row>
-    <row r="230" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="230" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E230" s="13"/>
       <c r="F230" s="14"/>
       <c r="G230" s="14"/>
@@ -3056,7 +3057,7 @@
       <c r="J230" s="15"/>
       <c r="K230" s="16"/>
     </row>
-    <row r="231" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="231" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E231" s="13"/>
       <c r="F231" s="14"/>
       <c r="G231" s="14"/>
@@ -3065,7 +3066,7 @@
       <c r="J231" s="15"/>
       <c r="K231" s="16"/>
     </row>
-    <row r="232" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="232" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E232" s="13"/>
       <c r="F232" s="14"/>
       <c r="G232" s="14"/>
@@ -3074,7 +3075,7 @@
       <c r="J232" s="15"/>
       <c r="K232" s="16"/>
     </row>
-    <row r="233" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="233" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E233" s="13"/>
       <c r="F233" s="14"/>
       <c r="G233" s="14"/>
@@ -3083,7 +3084,7 @@
       <c r="J233" s="15"/>
       <c r="K233" s="16"/>
     </row>
-    <row r="234" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="234" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E234" s="13"/>
       <c r="F234" s="14"/>
       <c r="G234" s="14"/>
@@ -3092,7 +3093,7 @@
       <c r="J234" s="15"/>
       <c r="K234" s="16"/>
     </row>
-    <row r="235" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="235" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E235" s="13"/>
       <c r="F235" s="14"/>
       <c r="G235" s="14"/>
@@ -3101,7 +3102,7 @@
       <c r="J235" s="15"/>
       <c r="K235" s="16"/>
     </row>
-    <row r="236" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="236" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E236" s="13"/>
       <c r="F236" s="14"/>
       <c r="G236" s="14"/>
@@ -3110,7 +3111,7 @@
       <c r="J236" s="15"/>
       <c r="K236" s="16"/>
     </row>
-    <row r="237" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="237" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E237" s="13"/>
       <c r="F237" s="14"/>
       <c r="G237" s="14"/>
@@ -3119,7 +3120,7 @@
       <c r="J237" s="15"/>
       <c r="K237" s="16"/>
     </row>
-    <row r="238" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="238" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E238" s="13"/>
       <c r="F238" s="14"/>
       <c r="G238" s="14"/>
@@ -3128,7 +3129,7 @@
       <c r="J238" s="15"/>
       <c r="K238" s="16"/>
     </row>
-    <row r="239" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="239" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E239" s="13"/>
       <c r="F239" s="14"/>
       <c r="G239" s="14"/>
@@ -3137,7 +3138,7 @@
       <c r="J239" s="15"/>
       <c r="K239" s="16"/>
     </row>
-    <row r="240" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="240" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E240" s="13"/>
       <c r="F240" s="14"/>
       <c r="G240" s="14"/>
@@ -3146,7 +3147,7 @@
       <c r="J240" s="15"/>
       <c r="K240" s="16"/>
     </row>
-    <row r="241" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="241" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E241" s="13"/>
       <c r="F241" s="14"/>
       <c r="G241" s="14"/>
@@ -3155,7 +3156,7 @@
       <c r="J241" s="15"/>
       <c r="K241" s="16"/>
     </row>
-    <row r="242" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="242" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E242" s="13"/>
       <c r="F242" s="14"/>
       <c r="G242" s="14"/>
@@ -3164,7 +3165,7 @@
       <c r="J242" s="15"/>
       <c r="K242" s="16"/>
     </row>
-    <row r="243" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="243" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E243" s="13"/>
       <c r="F243" s="14"/>
       <c r="G243" s="14"/>
@@ -3173,7 +3174,7 @@
       <c r="J243" s="15"/>
       <c r="K243" s="16"/>
     </row>
-    <row r="244" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="244" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E244" s="13"/>
       <c r="F244" s="14"/>
       <c r="G244" s="14"/>
@@ -3182,7 +3183,7 @@
       <c r="J244" s="15"/>
       <c r="K244" s="16"/>
     </row>
-    <row r="245" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="245" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E245" s="13"/>
       <c r="F245" s="14"/>
       <c r="G245" s="14"/>
@@ -3191,7 +3192,7 @@
       <c r="J245" s="15"/>
       <c r="K245" s="16"/>
     </row>
-    <row r="246" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="246" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E246" s="13"/>
       <c r="F246" s="14"/>
       <c r="G246" s="14"/>
@@ -3200,7 +3201,7 @@
       <c r="J246" s="15"/>
       <c r="K246" s="16"/>
     </row>
-    <row r="247" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="247" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E247" s="13"/>
       <c r="F247" s="14"/>
       <c r="G247" s="14"/>
@@ -3209,7 +3210,7 @@
       <c r="J247" s="15"/>
       <c r="K247" s="16"/>
     </row>
-    <row r="248" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="248" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E248" s="13"/>
       <c r="F248" s="14"/>
       <c r="G248" s="14"/>
@@ -3218,7 +3219,7 @@
       <c r="J248" s="15"/>
       <c r="K248" s="16"/>
     </row>
-    <row r="249" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="249" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E249" s="13"/>
       <c r="F249" s="14"/>
       <c r="G249" s="14"/>
@@ -3227,7 +3228,7 @@
       <c r="J249" s="15"/>
       <c r="K249" s="16"/>
     </row>
-    <row r="250" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="250" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E250" s="13"/>
       <c r="F250" s="14"/>
       <c r="G250" s="14"/>
@@ -3236,7 +3237,7 @@
       <c r="J250" s="15"/>
       <c r="K250" s="16"/>
     </row>
-    <row r="251" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="251" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E251" s="13"/>
       <c r="F251" s="14"/>
       <c r="G251" s="14"/>
@@ -3245,7 +3246,7 @@
       <c r="J251" s="15"/>
       <c r="K251" s="16"/>
     </row>
-    <row r="252" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="252" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E252" s="13"/>
       <c r="F252" s="14"/>
       <c r="G252" s="14"/>
@@ -3254,7 +3255,7 @@
       <c r="J252" s="15"/>
       <c r="K252" s="16"/>
     </row>
-    <row r="253" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="253" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E253" s="13"/>
       <c r="F253" s="14"/>
       <c r="G253" s="14"/>
@@ -3263,7 +3264,7 @@
       <c r="J253" s="15"/>
       <c r="K253" s="16"/>
     </row>
-    <row r="254" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="254" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E254" s="13"/>
       <c r="F254" s="14"/>
       <c r="G254" s="14"/>
@@ -3272,7 +3273,7 @@
       <c r="J254" s="15"/>
       <c r="K254" s="16"/>
     </row>
-    <row r="255" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="255" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E255" s="13"/>
       <c r="F255" s="14"/>
       <c r="G255" s="14"/>
@@ -3281,7 +3282,7 @@
       <c r="J255" s="15"/>
       <c r="K255" s="16"/>
     </row>
-    <row r="256" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="256" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E256" s="13"/>
       <c r="F256" s="14"/>
       <c r="G256" s="14"/>
@@ -3290,7 +3291,7 @@
       <c r="J256" s="15"/>
       <c r="K256" s="16"/>
     </row>
-    <row r="257" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="257" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E257" s="13"/>
       <c r="F257" s="14"/>
       <c r="G257" s="14"/>
@@ -3299,7 +3300,7 @@
       <c r="J257" s="15"/>
       <c r="K257" s="16"/>
     </row>
-    <row r="258" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="258" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E258" s="13"/>
       <c r="F258" s="14"/>
       <c r="G258" s="14"/>
@@ -3308,7 +3309,7 @@
       <c r="J258" s="15"/>
       <c r="K258" s="16"/>
     </row>
-    <row r="259" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="259" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E259" s="13"/>
       <c r="F259" s="14"/>
       <c r="G259" s="14"/>
@@ -3317,7 +3318,7 @@
       <c r="J259" s="15"/>
       <c r="K259" s="16"/>
     </row>
-    <row r="260" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="260" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E260" s="13"/>
       <c r="F260" s="14"/>
       <c r="G260" s="14"/>
@@ -3326,7 +3327,7 @@
       <c r="J260" s="15"/>
       <c r="K260" s="16"/>
     </row>
-    <row r="261" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="261" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E261" s="13"/>
       <c r="F261" s="14"/>
       <c r="G261" s="14"/>
@@ -3335,7 +3336,7 @@
       <c r="J261" s="15"/>
       <c r="K261" s="16"/>
     </row>
-    <row r="262" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="262" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E262" s="13"/>
       <c r="F262" s="14"/>
       <c r="G262" s="14"/>
@@ -3344,7 +3345,7 @@
       <c r="J262" s="15"/>
       <c r="K262" s="16"/>
     </row>
-    <row r="263" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="263" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E263" s="13"/>
       <c r="F263" s="14"/>
       <c r="G263" s="14"/>
@@ -3353,7 +3354,7 @@
       <c r="J263" s="15"/>
       <c r="K263" s="16"/>
     </row>
-    <row r="264" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="264" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E264" s="13"/>
       <c r="F264" s="14"/>
       <c r="G264" s="14"/>
@@ -3362,7 +3363,7 @@
       <c r="J264" s="15"/>
       <c r="K264" s="16"/>
     </row>
-    <row r="265" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="265" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E265" s="13"/>
       <c r="F265" s="14"/>
       <c r="G265" s="14"/>
@@ -3371,7 +3372,7 @@
       <c r="J265" s="15"/>
       <c r="K265" s="16"/>
     </row>
-    <row r="266" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="266" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E266" s="13"/>
       <c r="F266" s="14"/>
       <c r="G266" s="14"/>
@@ -3380,7 +3381,7 @@
       <c r="J266" s="15"/>
       <c r="K266" s="16"/>
     </row>
-    <row r="267" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="267" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E267" s="13"/>
       <c r="F267" s="14"/>
       <c r="G267" s="14"/>
@@ -3389,7 +3390,7 @@
       <c r="J267" s="15"/>
       <c r="K267" s="16"/>
     </row>
-    <row r="268" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="268" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E268" s="13"/>
       <c r="F268" s="14"/>
       <c r="G268" s="14"/>
@@ -3398,7 +3399,7 @@
       <c r="J268" s="15"/>
       <c r="K268" s="16"/>
     </row>
-    <row r="269" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="269" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E269" s="13"/>
       <c r="F269" s="14"/>
       <c r="G269" s="14"/>
@@ -3407,7 +3408,7 @@
       <c r="J269" s="15"/>
       <c r="K269" s="16"/>
     </row>
-    <row r="270" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="270" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E270" s="13"/>
       <c r="F270" s="14"/>
       <c r="G270" s="14"/>
@@ -3416,7 +3417,7 @@
       <c r="J270" s="15"/>
       <c r="K270" s="16"/>
     </row>
-    <row r="271" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="271" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E271" s="13"/>
       <c r="F271" s="14"/>
       <c r="G271" s="14"/>
@@ -3425,7 +3426,7 @@
       <c r="J271" s="15"/>
       <c r="K271" s="16"/>
     </row>
-    <row r="272" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="272" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E272" s="13"/>
       <c r="F272" s="14"/>
       <c r="G272" s="14"/>
@@ -3434,7 +3435,7 @@
       <c r="J272" s="15"/>
       <c r="K272" s="16"/>
     </row>
-    <row r="273" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="273" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E273" s="13"/>
       <c r="F273" s="14"/>
       <c r="G273" s="14"/>
@@ -3443,7 +3444,7 @@
       <c r="J273" s="15"/>
       <c r="K273" s="16"/>
     </row>
-    <row r="274" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="274" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E274" s="13"/>
       <c r="F274" s="14"/>
       <c r="G274" s="14"/>
@@ -3452,7 +3453,7 @@
       <c r="J274" s="15"/>
       <c r="K274" s="16"/>
     </row>
-    <row r="275" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="275" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E275" s="13"/>
       <c r="F275" s="14"/>
       <c r="G275" s="14"/>
@@ -3461,7 +3462,7 @@
       <c r="J275" s="15"/>
       <c r="K275" s="16"/>
     </row>
-    <row r="276" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="276" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E276" s="13"/>
       <c r="F276" s="14"/>
       <c r="G276" s="14"/>
@@ -3470,7 +3471,7 @@
       <c r="J276" s="15"/>
       <c r="K276" s="16"/>
     </row>
-    <row r="277" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="277" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E277" s="13"/>
       <c r="F277" s="14"/>
       <c r="G277" s="14"/>
@@ -3479,7 +3480,7 @@
       <c r="J277" s="15"/>
       <c r="K277" s="16"/>
     </row>
-    <row r="278" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="278" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E278" s="13"/>
       <c r="F278" s="14"/>
       <c r="G278" s="14"/>
@@ -3488,7 +3489,7 @@
       <c r="J278" s="15"/>
       <c r="K278" s="16"/>
     </row>
-    <row r="279" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="279" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E279" s="13"/>
       <c r="F279" s="14"/>
       <c r="G279" s="14"/>
@@ -3497,7 +3498,7 @@
       <c r="J279" s="15"/>
       <c r="K279" s="16"/>
     </row>
-    <row r="280" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="280" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E280" s="13"/>
       <c r="F280" s="14"/>
       <c r="G280" s="14"/>
@@ -3506,7 +3507,7 @@
       <c r="J280" s="15"/>
       <c r="K280" s="16"/>
     </row>
-    <row r="281" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="281" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E281" s="13"/>
       <c r="F281" s="14"/>
       <c r="G281" s="14"/>
@@ -3515,7 +3516,7 @@
       <c r="J281" s="15"/>
       <c r="K281" s="16"/>
     </row>
-    <row r="282" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="282" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E282" s="13"/>
       <c r="F282" s="14"/>
       <c r="G282" s="14"/>
@@ -3524,7 +3525,7 @@
       <c r="J282" s="15"/>
       <c r="K282" s="16"/>
     </row>
-    <row r="283" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="283" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E283" s="13"/>
       <c r="F283" s="14"/>
       <c r="G283" s="14"/>
@@ -3533,7 +3534,7 @@
       <c r="J283" s="15"/>
       <c r="K283" s="16"/>
     </row>
-    <row r="284" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="284" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E284" s="13"/>
       <c r="F284" s="14"/>
       <c r="G284" s="14"/>
@@ -3542,7 +3543,7 @@
       <c r="J284" s="15"/>
       <c r="K284" s="16"/>
     </row>
-    <row r="285" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="285" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E285" s="13"/>
       <c r="F285" s="14"/>
       <c r="G285" s="14"/>
@@ -3551,7 +3552,7 @@
       <c r="J285" s="15"/>
       <c r="K285" s="16"/>
     </row>
-    <row r="286" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="286" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E286" s="13"/>
       <c r="F286" s="14"/>
       <c r="G286" s="14"/>
@@ -3560,7 +3561,7 @@
       <c r="J286" s="15"/>
       <c r="K286" s="16"/>
     </row>
-    <row r="287" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="287" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E287" s="13"/>
       <c r="F287" s="14"/>
       <c r="G287" s="14"/>
@@ -3569,7 +3570,7 @@
       <c r="J287" s="15"/>
       <c r="K287" s="16"/>
     </row>
-    <row r="288" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="288" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E288" s="13"/>
       <c r="F288" s="14"/>
       <c r="G288" s="14"/>
@@ -3578,7 +3579,7 @@
       <c r="J288" s="15"/>
       <c r="K288" s="16"/>
     </row>
-    <row r="289" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="289" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E289" s="13"/>
       <c r="F289" s="14"/>
       <c r="G289" s="14"/>
@@ -3587,7 +3588,7 @@
       <c r="J289" s="15"/>
       <c r="K289" s="16"/>
     </row>
-    <row r="290" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="290" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E290" s="13"/>
       <c r="F290" s="14"/>
       <c r="G290" s="14"/>
@@ -3596,7 +3597,7 @@
       <c r="J290" s="15"/>
       <c r="K290" s="16"/>
     </row>
-    <row r="291" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="291" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E291" s="13"/>
       <c r="F291" s="14"/>
       <c r="G291" s="14"/>
@@ -3605,7 +3606,7 @@
       <c r="J291" s="15"/>
       <c r="K291" s="16"/>
     </row>
-    <row r="292" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="292" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E292" s="13"/>
       <c r="F292" s="14"/>
       <c r="G292" s="14"/>
@@ -3614,7 +3615,7 @@
       <c r="J292" s="15"/>
       <c r="K292" s="16"/>
     </row>
-    <row r="293" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="293" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E293" s="13"/>
       <c r="F293" s="14"/>
       <c r="G293" s="14"/>
@@ -3623,7 +3624,7 @@
       <c r="J293" s="15"/>
       <c r="K293" s="16"/>
     </row>
-    <row r="294" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="294" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E294" s="13"/>
       <c r="F294" s="14"/>
       <c r="G294" s="14"/>
@@ -3632,7 +3633,7 @@
       <c r="J294" s="15"/>
       <c r="K294" s="16"/>
     </row>
-    <row r="295" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="295" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E295" s="13"/>
       <c r="F295" s="14"/>
       <c r="G295" s="14"/>
@@ -3641,7 +3642,7 @@
       <c r="J295" s="15"/>
       <c r="K295" s="16"/>
     </row>
-    <row r="296" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="296" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E296" s="13"/>
       <c r="F296" s="14"/>
       <c r="G296" s="14"/>
@@ -3650,7 +3651,7 @@
       <c r="J296" s="15"/>
       <c r="K296" s="16"/>
     </row>
-    <row r="297" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="297" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E297" s="13"/>
       <c r="F297" s="14"/>
       <c r="G297" s="14"/>
@@ -3659,7 +3660,7 @@
       <c r="J297" s="15"/>
       <c r="K297" s="16"/>
     </row>
-    <row r="298" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="298" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E298" s="13"/>
       <c r="F298" s="14"/>
       <c r="G298" s="14"/>
@@ -3668,7 +3669,7 @@
       <c r="J298" s="15"/>
       <c r="K298" s="16"/>
     </row>
-    <row r="299" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="299" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E299" s="13"/>
       <c r="F299" s="14"/>
       <c r="G299" s="14"/>
@@ -3677,7 +3678,7 @@
       <c r="J299" s="15"/>
       <c r="K299" s="16"/>
     </row>
-    <row r="300" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="300" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E300" s="13"/>
       <c r="F300" s="14"/>
       <c r="G300" s="14"/>
@@ -3686,7 +3687,7 @@
       <c r="J300" s="15"/>
       <c r="K300" s="16"/>
     </row>
-    <row r="301" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="301" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E301" s="13"/>
       <c r="F301" s="14"/>
       <c r="G301" s="14"/>
@@ -3695,7 +3696,7 @@
       <c r="J301" s="15"/>
       <c r="K301" s="16"/>
     </row>
-    <row r="302" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="302" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E302" s="13"/>
       <c r="F302" s="14"/>
       <c r="G302" s="14"/>
@@ -3704,7 +3705,7 @@
       <c r="J302" s="15"/>
       <c r="K302" s="16"/>
     </row>
-    <row r="303" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="303" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E303" s="13"/>
       <c r="F303" s="14"/>
       <c r="G303" s="14"/>
@@ -3713,7 +3714,7 @@
       <c r="J303" s="15"/>
       <c r="K303" s="16"/>
     </row>
-    <row r="304" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="304" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E304" s="13"/>
       <c r="F304" s="14"/>
       <c r="G304" s="14"/>
@@ -3722,7 +3723,7 @@
       <c r="J304" s="15"/>
       <c r="K304" s="16"/>
     </row>
-    <row r="305" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="305" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E305" s="13"/>
       <c r="F305" s="14"/>
       <c r="G305" s="14"/>
@@ -3731,7 +3732,7 @@
       <c r="J305" s="15"/>
       <c r="K305" s="16"/>
     </row>
-    <row r="306" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="306" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E306" s="13"/>
       <c r="F306" s="14"/>
       <c r="G306" s="14"/>
@@ -3740,7 +3741,7 @@
       <c r="J306" s="15"/>
       <c r="K306" s="16"/>
     </row>
-    <row r="307" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="307" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E307" s="13"/>
       <c r="F307" s="14"/>
       <c r="G307" s="14"/>
@@ -3749,7 +3750,7 @@
       <c r="J307" s="15"/>
       <c r="K307" s="16"/>
     </row>
-    <row r="308" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="308" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E308" s="13"/>
       <c r="F308" s="14"/>
       <c r="G308" s="14"/>
@@ -3758,7 +3759,7 @@
       <c r="J308" s="15"/>
       <c r="K308" s="16"/>
     </row>
-    <row r="309" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="309" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E309" s="13"/>
       <c r="F309" s="14"/>
       <c r="G309" s="14"/>
@@ -3767,7 +3768,7 @@
       <c r="J309" s="15"/>
       <c r="K309" s="16"/>
     </row>
-    <row r="310" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="310" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E310" s="13"/>
       <c r="F310" s="14"/>
       <c r="G310" s="14"/>
@@ -3776,7 +3777,7 @@
       <c r="J310" s="15"/>
       <c r="K310" s="16"/>
     </row>
-    <row r="311" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="311" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E311" s="13"/>
       <c r="F311" s="14"/>
       <c r="G311" s="14"/>
@@ -3785,7 +3786,7 @@
       <c r="J311" s="15"/>
       <c r="K311" s="16"/>
     </row>
-    <row r="312" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="312" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E312" s="13"/>
       <c r="F312" s="14"/>
       <c r="G312" s="14"/>
@@ -3794,7 +3795,7 @@
       <c r="J312" s="15"/>
       <c r="K312" s="16"/>
     </row>
-    <row r="313" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="313" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E313" s="13"/>
       <c r="F313" s="14"/>
       <c r="G313" s="14"/>
@@ -3803,7 +3804,7 @@
       <c r="J313" s="15"/>
       <c r="K313" s="16"/>
     </row>
-    <row r="314" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="314" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E314" s="13"/>
       <c r="F314" s="14"/>
       <c r="G314" s="14"/>
@@ -3812,7 +3813,7 @@
       <c r="J314" s="15"/>
       <c r="K314" s="16"/>
     </row>
-    <row r="315" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="315" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E315" s="13"/>
       <c r="F315" s="14"/>
       <c r="G315" s="14"/>
@@ -3821,7 +3822,7 @@
       <c r="J315" s="15"/>
       <c r="K315" s="16"/>
     </row>
-    <row r="316" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="316" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E316" s="13"/>
       <c r="F316" s="14"/>
       <c r="G316" s="14"/>
@@ -3830,7 +3831,7 @@
       <c r="J316" s="15"/>
       <c r="K316" s="16"/>
     </row>
-    <row r="317" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="317" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E317" s="13"/>
       <c r="F317" s="14"/>
       <c r="G317" s="14"/>
@@ -3839,7 +3840,7 @@
       <c r="J317" s="15"/>
       <c r="K317" s="16"/>
     </row>
-    <row r="318" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="318" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E318" s="13"/>
       <c r="F318" s="14"/>
       <c r="G318" s="14"/>
@@ -3848,7 +3849,7 @@
       <c r="J318" s="15"/>
       <c r="K318" s="16"/>
     </row>
-    <row r="319" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="319" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E319" s="13"/>
       <c r="F319" s="14"/>
       <c r="G319" s="14"/>
@@ -3857,7 +3858,7 @@
       <c r="J319" s="15"/>
       <c r="K319" s="16"/>
     </row>
-    <row r="320" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="320" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E320" s="13"/>
       <c r="F320" s="14"/>
       <c r="G320" s="14"/>
@@ -3866,7 +3867,7 @@
       <c r="J320" s="15"/>
       <c r="K320" s="16"/>
     </row>
-    <row r="321" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="321" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E321" s="13"/>
       <c r="F321" s="14"/>
       <c r="G321" s="14"/>
@@ -3875,7 +3876,7 @@
       <c r="J321" s="15"/>
       <c r="K321" s="16"/>
     </row>
-    <row r="322" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="322" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E322" s="13"/>
       <c r="F322" s="14"/>
       <c r="G322" s="14"/>
@@ -3884,7 +3885,7 @@
       <c r="J322" s="15"/>
       <c r="K322" s="16"/>
     </row>
-    <row r="323" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="323" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E323" s="13"/>
       <c r="F323" s="14"/>
       <c r="G323" s="14"/>
@@ -3893,7 +3894,7 @@
       <c r="J323" s="15"/>
       <c r="K323" s="16"/>
     </row>
-    <row r="324" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="324" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E324" s="13"/>
       <c r="F324" s="14"/>
       <c r="G324" s="14"/>
@@ -3902,7 +3903,7 @@
       <c r="J324" s="15"/>
       <c r="K324" s="16"/>
     </row>
-    <row r="325" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="325" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E325" s="13"/>
       <c r="F325" s="14"/>
       <c r="G325" s="14"/>
@@ -3911,7 +3912,7 @@
       <c r="J325" s="15"/>
       <c r="K325" s="16"/>
     </row>
-    <row r="326" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="326" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E326" s="13"/>
       <c r="F326" s="14"/>
       <c r="G326" s="14"/>
@@ -3920,7 +3921,7 @@
       <c r="J326" s="15"/>
       <c r="K326" s="16"/>
     </row>
-    <row r="327" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="327" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E327" s="13"/>
       <c r="F327" s="14"/>
       <c r="G327" s="14"/>
@@ -3929,7 +3930,7 @@
       <c r="J327" s="15"/>
       <c r="K327" s="16"/>
     </row>
-    <row r="328" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="328" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E328" s="13"/>
       <c r="F328" s="14"/>
       <c r="G328" s="14"/>
@@ -3938,7 +3939,7 @@
       <c r="J328" s="15"/>
       <c r="K328" s="16"/>
     </row>
-    <row r="329" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="329" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E329" s="13"/>
       <c r="F329" s="14"/>
       <c r="G329" s="14"/>
@@ -3947,7 +3948,7 @@
       <c r="J329" s="15"/>
       <c r="K329" s="16"/>
     </row>
-    <row r="330" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="330" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E330" s="13"/>
       <c r="F330" s="14"/>
       <c r="G330" s="14"/>
@@ -3956,7 +3957,7 @@
       <c r="J330" s="15"/>
       <c r="K330" s="16"/>
     </row>
-    <row r="331" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="331" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E331" s="13"/>
       <c r="F331" s="14"/>
       <c r="G331" s="14"/>
@@ -3965,7 +3966,7 @@
       <c r="J331" s="15"/>
       <c r="K331" s="16"/>
     </row>
-    <row r="332" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="332" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E332" s="13"/>
       <c r="F332" s="14"/>
       <c r="G332" s="14"/>
@@ -3974,7 +3975,7 @@
       <c r="J332" s="15"/>
       <c r="K332" s="16"/>
     </row>
-    <row r="333" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="333" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E333" s="13"/>
       <c r="F333" s="14"/>
       <c r="G333" s="14"/>
@@ -3983,7 +3984,7 @@
       <c r="J333" s="15"/>
       <c r="K333" s="16"/>
     </row>
-    <row r="334" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="334" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E334" s="13"/>
       <c r="F334" s="14"/>
       <c r="G334" s="14"/>
@@ -3992,7 +3993,7 @@
       <c r="J334" s="15"/>
       <c r="K334" s="16"/>
     </row>
-    <row r="335" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="335" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E335" s="13"/>
       <c r="F335" s="14"/>
       <c r="G335" s="14"/>
@@ -4001,7 +4002,7 @@
       <c r="J335" s="15"/>
       <c r="K335" s="16"/>
     </row>
-    <row r="336" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="336" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E336" s="13"/>
       <c r="F336" s="14"/>
       <c r="G336" s="14"/>
@@ -4010,7 +4011,7 @@
       <c r="J336" s="15"/>
       <c r="K336" s="16"/>
     </row>
-    <row r="337" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="337" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E337" s="13"/>
       <c r="F337" s="14"/>
       <c r="G337" s="14"/>
@@ -4019,7 +4020,7 @@
       <c r="J337" s="15"/>
       <c r="K337" s="16"/>
     </row>
-    <row r="338" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="338" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E338" s="13"/>
       <c r="F338" s="14"/>
       <c r="G338" s="14"/>
@@ -4028,7 +4029,7 @@
       <c r="J338" s="15"/>
       <c r="K338" s="16"/>
     </row>
-    <row r="339" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="339" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E339" s="13"/>
       <c r="F339" s="14"/>
       <c r="G339" s="14"/>
@@ -4037,7 +4038,7 @@
       <c r="J339" s="15"/>
       <c r="K339" s="16"/>
     </row>
-    <row r="340" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="340" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E340" s="13"/>
       <c r="F340" s="14"/>
       <c r="G340" s="14"/>
@@ -4046,7 +4047,7 @@
       <c r="J340" s="15"/>
       <c r="K340" s="16"/>
     </row>
-    <row r="341" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="341" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E341" s="13"/>
       <c r="F341" s="14"/>
       <c r="G341" s="14"/>
@@ -4055,7 +4056,7 @@
       <c r="J341" s="15"/>
       <c r="K341" s="16"/>
     </row>
-    <row r="342" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="342" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E342" s="13"/>
       <c r="F342" s="14"/>
       <c r="G342" s="14"/>
@@ -4064,7 +4065,7 @@
       <c r="J342" s="15"/>
       <c r="K342" s="16"/>
     </row>
-    <row r="343" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="343" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E343" s="13"/>
       <c r="F343" s="14"/>
       <c r="G343" s="14"/>
@@ -4073,7 +4074,7 @@
       <c r="J343" s="15"/>
       <c r="K343" s="16"/>
     </row>
-    <row r="344" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="344" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E344" s="13"/>
       <c r="F344" s="14"/>
       <c r="G344" s="14"/>
@@ -4082,7 +4083,7 @@
       <c r="J344" s="15"/>
       <c r="K344" s="16"/>
     </row>
-    <row r="345" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="345" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E345" s="13"/>
       <c r="F345" s="14"/>
       <c r="G345" s="14"/>
@@ -4091,7 +4092,7 @@
       <c r="J345" s="15"/>
       <c r="K345" s="16"/>
     </row>
-    <row r="346" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="346" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E346" s="13"/>
       <c r="F346" s="14"/>
       <c r="G346" s="14"/>
@@ -4100,7 +4101,7 @@
       <c r="J346" s="15"/>
       <c r="K346" s="16"/>
     </row>
-    <row r="347" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="347" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E347" s="13"/>
       <c r="F347" s="14"/>
       <c r="G347" s="14"/>
@@ -4109,7 +4110,7 @@
       <c r="J347" s="15"/>
       <c r="K347" s="16"/>
     </row>
-    <row r="348" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="348" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E348" s="13"/>
       <c r="F348" s="14"/>
       <c r="G348" s="14"/>
@@ -4118,7 +4119,7 @@
       <c r="J348" s="15"/>
       <c r="K348" s="16"/>
     </row>
-    <row r="349" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="349" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E349" s="13"/>
       <c r="F349" s="14"/>
       <c r="G349" s="14"/>
@@ -4127,7 +4128,7 @@
       <c r="J349" s="15"/>
       <c r="K349" s="16"/>
     </row>
-    <row r="350" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="350" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E350" s="13"/>
       <c r="F350" s="14"/>
       <c r="G350" s="14"/>
@@ -4136,7 +4137,7 @@
       <c r="J350" s="15"/>
       <c r="K350" s="16"/>
     </row>
-    <row r="351" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="351" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E351" s="13"/>
       <c r="F351" s="14"/>
       <c r="G351" s="14"/>
@@ -4145,7 +4146,7 @@
       <c r="J351" s="15"/>
       <c r="K351" s="16"/>
     </row>
-    <row r="352" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="352" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E352" s="13"/>
       <c r="F352" s="14"/>
       <c r="G352" s="14"/>
@@ -4154,7 +4155,7 @@
       <c r="J352" s="15"/>
       <c r="K352" s="16"/>
     </row>
-    <row r="353" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="353" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E353" s="13"/>
       <c r="F353" s="14"/>
       <c r="G353" s="14"/>
@@ -4163,7 +4164,7 @@
       <c r="J353" s="15"/>
       <c r="K353" s="16"/>
     </row>
-    <row r="354" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="354" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E354" s="13"/>
       <c r="F354" s="14"/>
       <c r="G354" s="14"/>
@@ -4172,7 +4173,7 @@
       <c r="J354" s="15"/>
       <c r="K354" s="16"/>
     </row>
-    <row r="355" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="355" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E355" s="13"/>
       <c r="F355" s="14"/>
       <c r="G355" s="14"/>
@@ -4181,7 +4182,7 @@
       <c r="J355" s="15"/>
       <c r="K355" s="16"/>
     </row>
-    <row r="356" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="356" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E356" s="13"/>
       <c r="F356" s="14"/>
       <c r="G356" s="14"/>
@@ -4190,7 +4191,7 @@
       <c r="J356" s="15"/>
       <c r="K356" s="16"/>
     </row>
-    <row r="357" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="357" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E357" s="13"/>
       <c r="F357" s="14"/>
       <c r="G357" s="14"/>
@@ -4199,7 +4200,7 @@
       <c r="J357" s="15"/>
       <c r="K357" s="16"/>
     </row>
-    <row r="358" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="358" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E358" s="13"/>
       <c r="F358" s="14"/>
       <c r="G358" s="14"/>
@@ -4208,7 +4209,7 @@
       <c r="J358" s="15"/>
       <c r="K358" s="16"/>
     </row>
-    <row r="359" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="359" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E359" s="13"/>
       <c r="F359" s="14"/>
       <c r="G359" s="14"/>
@@ -4217,7 +4218,7 @@
       <c r="J359" s="15"/>
       <c r="K359" s="16"/>
     </row>
-    <row r="360" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="360" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E360" s="13"/>
       <c r="F360" s="14"/>
       <c r="G360" s="14"/>
@@ -4226,7 +4227,7 @@
       <c r="J360" s="15"/>
       <c r="K360" s="16"/>
     </row>
-    <row r="361" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="361" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E361" s="13"/>
       <c r="F361" s="14"/>
       <c r="G361" s="14"/>
@@ -4235,7 +4236,7 @@
       <c r="J361" s="15"/>
       <c r="K361" s="16"/>
     </row>
-    <row r="362" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="362" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E362" s="13"/>
       <c r="F362" s="14"/>
       <c r="G362" s="14"/>
@@ -4244,7 +4245,7 @@
       <c r="J362" s="15"/>
       <c r="K362" s="16"/>
     </row>
-    <row r="363" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="363" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E363" s="13"/>
       <c r="F363" s="14"/>
       <c r="G363" s="14"/>
@@ -4253,7 +4254,7 @@
       <c r="J363" s="15"/>
       <c r="K363" s="16"/>
     </row>
-    <row r="364" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="364" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E364" s="13"/>
       <c r="F364" s="14"/>
       <c r="G364" s="14"/>
@@ -4262,7 +4263,7 @@
       <c r="J364" s="15"/>
       <c r="K364" s="16"/>
     </row>
-    <row r="365" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="365" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E365" s="13"/>
       <c r="F365" s="14"/>
       <c r="G365" s="14"/>
@@ -4271,7 +4272,7 @@
       <c r="J365" s="15"/>
       <c r="K365" s="16"/>
     </row>
-    <row r="366" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="366" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E366" s="13"/>
       <c r="F366" s="14"/>
       <c r="G366" s="14"/>
@@ -4280,7 +4281,7 @@
       <c r="J366" s="15"/>
       <c r="K366" s="16"/>
     </row>
-    <row r="367" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="367" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E367" s="13"/>
       <c r="F367" s="14"/>
       <c r="G367" s="14"/>
@@ -4289,7 +4290,7 @@
       <c r="J367" s="15"/>
       <c r="K367" s="16"/>
     </row>
-    <row r="368" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="368" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E368" s="13"/>
       <c r="F368" s="14"/>
       <c r="G368" s="14"/>
@@ -4298,7 +4299,7 @@
       <c r="J368" s="15"/>
       <c r="K368" s="16"/>
     </row>
-    <row r="369" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="369" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E369" s="13"/>
       <c r="F369" s="14"/>
       <c r="G369" s="14"/>
@@ -4307,7 +4308,7 @@
       <c r="J369" s="15"/>
       <c r="K369" s="16"/>
     </row>
-    <row r="370" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="370" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E370" s="13"/>
       <c r="F370" s="14"/>
       <c r="G370" s="14"/>
@@ -4316,7 +4317,7 @@
       <c r="J370" s="15"/>
       <c r="K370" s="16"/>
     </row>
-    <row r="371" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="371" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E371" s="13"/>
       <c r="F371" s="14"/>
       <c r="G371" s="14"/>
@@ -4325,7 +4326,7 @@
       <c r="J371" s="15"/>
       <c r="K371" s="16"/>
     </row>
-    <row r="372" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="372" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E372" s="13"/>
       <c r="F372" s="14"/>
       <c r="G372" s="14"/>
@@ -4334,7 +4335,7 @@
       <c r="J372" s="15"/>
       <c r="K372" s="16"/>
     </row>
-    <row r="373" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="373" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E373" s="13"/>
       <c r="F373" s="14"/>
       <c r="G373" s="14"/>
@@ -4343,7 +4344,7 @@
       <c r="J373" s="15"/>
       <c r="K373" s="16"/>
     </row>
-    <row r="374" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="374" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E374" s="13"/>
       <c r="F374" s="14"/>
       <c r="G374" s="14"/>
@@ -4352,7 +4353,7 @@
       <c r="J374" s="15"/>
       <c r="K374" s="16"/>
     </row>
-    <row r="375" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="375" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E375" s="13"/>
       <c r="F375" s="14"/>
       <c r="G375" s="14"/>
@@ -4361,7 +4362,7 @@
       <c r="J375" s="15"/>
       <c r="K375" s="16"/>
     </row>
-    <row r="376" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="376" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E376" s="13"/>
       <c r="F376" s="14"/>
       <c r="G376" s="14"/>
@@ -4370,7 +4371,7 @@
       <c r="J376" s="15"/>
       <c r="K376" s="16"/>
     </row>
-    <row r="377" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="377" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E377" s="13"/>
       <c r="F377" s="14"/>
       <c r="G377" s="14"/>
@@ -4379,7 +4380,7 @@
       <c r="J377" s="15"/>
       <c r="K377" s="16"/>
     </row>
-    <row r="378" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="378" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E378" s="13"/>
       <c r="F378" s="14"/>
       <c r="G378" s="14"/>
@@ -4388,7 +4389,7 @@
       <c r="J378" s="15"/>
       <c r="K378" s="16"/>
     </row>
-    <row r="379" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="379" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E379" s="13"/>
       <c r="F379" s="14"/>
       <c r="G379" s="14"/>
@@ -4397,7 +4398,7 @@
       <c r="J379" s="15"/>
       <c r="K379" s="16"/>
     </row>
-    <row r="380" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="380" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E380" s="13"/>
       <c r="F380" s="14"/>
       <c r="G380" s="14"/>
@@ -4406,7 +4407,7 @@
       <c r="J380" s="15"/>
       <c r="K380" s="16"/>
     </row>
-    <row r="381" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="381" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E381" s="13"/>
       <c r="F381" s="14"/>
       <c r="G381" s="14"/>
@@ -4415,7 +4416,7 @@
       <c r="J381" s="15"/>
       <c r="K381" s="16"/>
     </row>
-    <row r="382" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="382" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E382" s="13"/>
       <c r="F382" s="14"/>
       <c r="G382" s="14"/>
@@ -4424,7 +4425,7 @@
       <c r="J382" s="15"/>
       <c r="K382" s="16"/>
     </row>
-    <row r="383" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="383" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E383" s="13"/>
       <c r="F383" s="14"/>
       <c r="G383" s="14"/>
@@ -4433,7 +4434,7 @@
       <c r="J383" s="15"/>
       <c r="K383" s="16"/>
     </row>
-    <row r="384" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="384" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E384" s="13"/>
       <c r="F384" s="14"/>
       <c r="G384" s="14"/>
@@ -4442,7 +4443,7 @@
       <c r="J384" s="15"/>
       <c r="K384" s="16"/>
     </row>
-    <row r="385" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="385" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E385" s="13"/>
       <c r="F385" s="14"/>
       <c r="G385" s="14"/>
@@ -4451,7 +4452,7 @@
       <c r="J385" s="15"/>
       <c r="K385" s="16"/>
     </row>
-    <row r="386" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="386" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E386" s="13"/>
       <c r="F386" s="14"/>
       <c r="G386" s="14"/>
@@ -4460,7 +4461,7 @@
       <c r="J386" s="15"/>
       <c r="K386" s="16"/>
     </row>
-    <row r="387" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="387" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E387" s="13"/>
       <c r="F387" s="14"/>
       <c r="G387" s="14"/>
@@ -4469,7 +4470,7 @@
       <c r="J387" s="15"/>
       <c r="K387" s="16"/>
     </row>
-    <row r="388" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="388" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E388" s="13"/>
       <c r="F388" s="14"/>
       <c r="G388" s="14"/>
@@ -4478,7 +4479,7 @@
       <c r="J388" s="15"/>
       <c r="K388" s="16"/>
     </row>
-    <row r="389" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="389" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E389" s="13"/>
       <c r="F389" s="14"/>
       <c r="G389" s="14"/>
@@ -4487,7 +4488,7 @@
       <c r="J389" s="15"/>
       <c r="K389" s="16"/>
     </row>
-    <row r="390" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="390" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E390" s="13"/>
       <c r="F390" s="14"/>
       <c r="G390" s="14"/>
@@ -4496,7 +4497,7 @@
       <c r="J390" s="15"/>
       <c r="K390" s="16"/>
     </row>
-    <row r="391" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="391" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E391" s="13"/>
       <c r="F391" s="14"/>
       <c r="G391" s="14"/>
@@ -4505,7 +4506,7 @@
       <c r="J391" s="15"/>
       <c r="K391" s="16"/>
     </row>
-    <row r="392" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="392" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E392" s="13"/>
       <c r="F392" s="14"/>
       <c r="G392" s="14"/>
@@ -4514,7 +4515,7 @@
       <c r="J392" s="15"/>
       <c r="K392" s="16"/>
     </row>
-    <row r="393" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="393" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E393" s="13"/>
       <c r="F393" s="14"/>
       <c r="G393" s="14"/>
@@ -4523,7 +4524,7 @@
       <c r="J393" s="15"/>
       <c r="K393" s="16"/>
     </row>
-    <row r="394" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="394" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E394" s="13"/>
       <c r="F394" s="14"/>
       <c r="G394" s="14"/>
@@ -4532,7 +4533,7 @@
       <c r="J394" s="15"/>
       <c r="K394" s="16"/>
     </row>
-    <row r="395" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="395" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E395" s="13"/>
       <c r="F395" s="14"/>
       <c r="G395" s="14"/>
@@ -4541,7 +4542,7 @@
       <c r="J395" s="15"/>
       <c r="K395" s="16"/>
     </row>
-    <row r="396" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="396" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E396" s="13"/>
       <c r="F396" s="14"/>
       <c r="G396" s="14"/>
@@ -4550,7 +4551,7 @@
       <c r="J396" s="15"/>
       <c r="K396" s="16"/>
     </row>
-    <row r="397" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="397" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E397" s="13"/>
       <c r="F397" s="14"/>
       <c r="G397" s="14"/>
@@ -4559,7 +4560,7 @@
       <c r="J397" s="15"/>
       <c r="K397" s="16"/>
     </row>
-    <row r="398" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="398" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E398" s="13"/>
       <c r="F398" s="14"/>
       <c r="G398" s="14"/>
@@ -4568,7 +4569,7 @@
       <c r="J398" s="15"/>
       <c r="K398" s="16"/>
     </row>
-    <row r="399" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="399" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E399" s="13"/>
       <c r="F399" s="14"/>
       <c r="G399" s="14"/>
@@ -4577,7 +4578,7 @@
       <c r="J399" s="15"/>
       <c r="K399" s="16"/>
     </row>
-    <row r="400" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="400" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E400" s="13"/>
       <c r="F400" s="14"/>
       <c r="G400" s="14"/>
@@ -4586,7 +4587,7 @@
       <c r="J400" s="15"/>
       <c r="K400" s="16"/>
     </row>
-    <row r="401" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="401" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E401" s="13"/>
       <c r="F401" s="14"/>
       <c r="G401" s="14"/>
@@ -4595,7 +4596,7 @@
       <c r="J401" s="15"/>
       <c r="K401" s="16"/>
     </row>
-    <row r="402" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="402" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E402" s="13"/>
       <c r="F402" s="14"/>
       <c r="G402" s="14"/>
@@ -4604,7 +4605,7 @@
       <c r="J402" s="15"/>
       <c r="K402" s="16"/>
     </row>
-    <row r="403" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="403" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E403" s="13"/>
       <c r="F403" s="14"/>
       <c r="G403" s="14"/>
@@ -4613,7 +4614,7 @@
       <c r="J403" s="15"/>
       <c r="K403" s="16"/>
     </row>
-    <row r="404" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="404" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E404" s="13"/>
       <c r="F404" s="14"/>
       <c r="G404" s="14"/>
@@ -4622,7 +4623,7 @@
       <c r="J404" s="15"/>
       <c r="K404" s="16"/>
     </row>
-    <row r="405" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="405" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E405" s="13"/>
       <c r="F405" s="14"/>
       <c r="G405" s="14"/>
@@ -4631,7 +4632,7 @@
       <c r="J405" s="15"/>
       <c r="K405" s="16"/>
     </row>
-    <row r="406" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="406" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E406" s="13"/>
       <c r="F406" s="14"/>
       <c r="G406" s="14"/>
@@ -4640,7 +4641,7 @@
       <c r="J406" s="15"/>
       <c r="K406" s="16"/>
     </row>
-    <row r="407" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="407" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E407" s="17"/>
       <c r="F407" s="18"/>
       <c r="G407" s="18"/>
@@ -4649,745 +4650,745 @@
       <c r="J407" s="19"/>
       <c r="K407" s="20"/>
     </row>
-    <row r="408" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="408" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K408" s="8"/>
     </row>
-    <row r="409" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="409" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K409" s="8"/>
     </row>
-    <row r="410" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="410" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K410" s="8"/>
     </row>
-    <row r="411" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="411" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K411" s="8"/>
     </row>
-    <row r="412" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="412" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K412" s="8"/>
     </row>
-    <row r="413" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="413" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K413" s="8"/>
     </row>
-    <row r="414" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="414" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K414" s="8"/>
     </row>
-    <row r="415" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="415" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K415" s="8"/>
     </row>
-    <row r="416" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="416" spans="5:11" x14ac:dyDescent="0.25">
       <c r="K416" s="8"/>
     </row>
-    <row r="417" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="417" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K417" s="8"/>
     </row>
-    <row r="418" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="418" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K418" s="8"/>
     </row>
-    <row r="419" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="419" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K419" s="8"/>
     </row>
-    <row r="420" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="420" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K420" s="8"/>
     </row>
-    <row r="421" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="421" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K421" s="8"/>
     </row>
-    <row r="422" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="422" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K422" s="8"/>
     </row>
-    <row r="423" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="423" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K423" s="8"/>
     </row>
-    <row r="424" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="424" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K424" s="8"/>
     </row>
-    <row r="425" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="425" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K425" s="8"/>
     </row>
-    <row r="426" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="426" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K426" s="8"/>
     </row>
-    <row r="427" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="427" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K427" s="8"/>
     </row>
-    <row r="428" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="428" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K428" s="8"/>
     </row>
-    <row r="429" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="429" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K429" s="8"/>
     </row>
-    <row r="430" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="430" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K430" s="8"/>
     </row>
-    <row r="431" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="431" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K431" s="8"/>
     </row>
-    <row r="432" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="432" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K432" s="8"/>
     </row>
-    <row r="433" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="433" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K433" s="8"/>
     </row>
-    <row r="434" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="434" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K434" s="8"/>
     </row>
-    <row r="435" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="435" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K435" s="8"/>
     </row>
-    <row r="436" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="436" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K436" s="8"/>
     </row>
-    <row r="437" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="437" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K437" s="8"/>
     </row>
-    <row r="438" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="438" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K438" s="8"/>
     </row>
-    <row r="439" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="439" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K439" s="8"/>
     </row>
-    <row r="440" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="440" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K440" s="8"/>
     </row>
-    <row r="441" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="441" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K441" s="8"/>
     </row>
-    <row r="442" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="442" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K442" s="8"/>
     </row>
-    <row r="443" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="443" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K443" s="8"/>
     </row>
-    <row r="444" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="444" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K444" s="8"/>
     </row>
-    <row r="445" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="445" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K445" s="8"/>
     </row>
-    <row r="446" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="446" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K446" s="8"/>
     </row>
-    <row r="447" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="447" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K447" s="8"/>
     </row>
-    <row r="448" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="448" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K448" s="8"/>
     </row>
-    <row r="449" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="449" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K449" s="8"/>
     </row>
-    <row r="450" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="450" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K450" s="8"/>
     </row>
-    <row r="451" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="451" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K451" s="8"/>
     </row>
-    <row r="452" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="452" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K452" s="8"/>
     </row>
-    <row r="453" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="453" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K453" s="8"/>
     </row>
-    <row r="454" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="454" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K454" s="8"/>
     </row>
-    <row r="455" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="455" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K455" s="8"/>
     </row>
-    <row r="456" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="456" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K456" s="8"/>
     </row>
-    <row r="457" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="457" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K457" s="8"/>
     </row>
-    <row r="458" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="458" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K458" s="8"/>
     </row>
-    <row r="459" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="459" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K459" s="8"/>
     </row>
-    <row r="460" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="460" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K460" s="8"/>
     </row>
-    <row r="461" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="461" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K461" s="8"/>
     </row>
-    <row r="462" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="462" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K462" s="8"/>
     </row>
-    <row r="463" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="463" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K463" s="8"/>
     </row>
-    <row r="464" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="464" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K464" s="8"/>
     </row>
-    <row r="465" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="465" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K465" s="8"/>
     </row>
-    <row r="466" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="466" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K466" s="8"/>
     </row>
-    <row r="467" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="467" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K467" s="8"/>
     </row>
-    <row r="468" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="468" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K468" s="8"/>
     </row>
-    <row r="469" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="469" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K469" s="8"/>
     </row>
-    <row r="470" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="470" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K470" s="8"/>
     </row>
-    <row r="471" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="471" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K471" s="8"/>
     </row>
-    <row r="472" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="472" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K472" s="8"/>
     </row>
-    <row r="473" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="473" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K473" s="8"/>
     </row>
-    <row r="474" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="474" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K474" s="8"/>
     </row>
-    <row r="475" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="475" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K475" s="8"/>
     </row>
-    <row r="476" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="476" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K476" s="8"/>
     </row>
-    <row r="477" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="477" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K477" s="8"/>
     </row>
-    <row r="478" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="478" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K478" s="8"/>
     </row>
-    <row r="479" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="479" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K479" s="8"/>
     </row>
-    <row r="480" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="480" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K480" s="8"/>
     </row>
-    <row r="481" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="481" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K481" s="8"/>
     </row>
-    <row r="482" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="482" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K482" s="8"/>
     </row>
-    <row r="483" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="483" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K483" s="8"/>
     </row>
-    <row r="484" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="484" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K484" s="8"/>
     </row>
-    <row r="485" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="485" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K485" s="8"/>
     </row>
-    <row r="486" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="486" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K486" s="8"/>
     </row>
-    <row r="487" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="487" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K487" s="8"/>
     </row>
-    <row r="488" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="488" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K488" s="8"/>
     </row>
-    <row r="489" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="489" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K489" s="8"/>
     </row>
-    <row r="490" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="490" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K490" s="8"/>
     </row>
-    <row r="491" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="491" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K491" s="8"/>
     </row>
-    <row r="492" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="492" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K492" s="8"/>
     </row>
-    <row r="493" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="493" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K493" s="8"/>
     </row>
-    <row r="494" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="494" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K494" s="8"/>
     </row>
-    <row r="495" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="495" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K495" s="8"/>
     </row>
-    <row r="496" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="496" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K496" s="8"/>
     </row>
-    <row r="497" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="497" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K497" s="8"/>
     </row>
-    <row r="498" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="498" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K498" s="8"/>
     </row>
-    <row r="499" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="499" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K499" s="8"/>
     </row>
-    <row r="500" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="500" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K500" s="8"/>
     </row>
-    <row r="501" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="501" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K501" s="8"/>
     </row>
-    <row r="502" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="502" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K502" s="8"/>
     </row>
-    <row r="503" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="503" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K503" s="8"/>
     </row>
-    <row r="504" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="504" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K504" s="8"/>
     </row>
-    <row r="505" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="505" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K505" s="8"/>
     </row>
-    <row r="506" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="506" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K506" s="8"/>
     </row>
-    <row r="507" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="507" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K507" s="8"/>
     </row>
-    <row r="508" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="508" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K508" s="8"/>
     </row>
-    <row r="509" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="509" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K509" s="8"/>
     </row>
-    <row r="510" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="510" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K510" s="8"/>
     </row>
-    <row r="511" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="511" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K511" s="8"/>
     </row>
-    <row r="512" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="512" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K512" s="8"/>
     </row>
-    <row r="513" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="513" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K513" s="8"/>
     </row>
-    <row r="514" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="514" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K514" s="8"/>
     </row>
-    <row r="515" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="515" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K515" s="8"/>
     </row>
-    <row r="516" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="516" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K516" s="8"/>
     </row>
-    <row r="517" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="517" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K517" s="8"/>
     </row>
-    <row r="518" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="518" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K518" s="8"/>
     </row>
-    <row r="519" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="519" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K519" s="8"/>
     </row>
-    <row r="520" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="520" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K520" s="8"/>
     </row>
-    <row r="521" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="521" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K521" s="8"/>
     </row>
-    <row r="522" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="522" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K522" s="8"/>
     </row>
-    <row r="523" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="523" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K523" s="8"/>
     </row>
-    <row r="524" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="524" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K524" s="8"/>
     </row>
-    <row r="525" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="525" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K525" s="8"/>
     </row>
-    <row r="526" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="526" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K526" s="8"/>
     </row>
-    <row r="527" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="527" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K527" s="8"/>
     </row>
-    <row r="528" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="528" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K528" s="8"/>
     </row>
-    <row r="529" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="529" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K529" s="8"/>
     </row>
-    <row r="530" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="530" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K530" s="8"/>
     </row>
-    <row r="531" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="531" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K531" s="8"/>
     </row>
-    <row r="532" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="532" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K532" s="8"/>
     </row>
-    <row r="533" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="533" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K533" s="8"/>
     </row>
-    <row r="534" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="534" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K534" s="8"/>
     </row>
-    <row r="535" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="535" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K535" s="8"/>
     </row>
-    <row r="536" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="536" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K536" s="8"/>
     </row>
-    <row r="537" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="537" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K537" s="8"/>
     </row>
-    <row r="538" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="538" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K538" s="8"/>
     </row>
-    <row r="539" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="539" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K539" s="8"/>
     </row>
-    <row r="540" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="540" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K540" s="8"/>
     </row>
-    <row r="541" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="541" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K541" s="8"/>
     </row>
-    <row r="542" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="542" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K542" s="8"/>
     </row>
-    <row r="543" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="543" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K543" s="8"/>
     </row>
-    <row r="544" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="544" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K544" s="8"/>
     </row>
-    <row r="545" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="545" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K545" s="8"/>
     </row>
-    <row r="546" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="546" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K546" s="8"/>
     </row>
-    <row r="547" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="547" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K547" s="8"/>
     </row>
-    <row r="548" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="548" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K548" s="8"/>
     </row>
-    <row r="549" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="549" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K549" s="8"/>
     </row>
-    <row r="550" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="550" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K550" s="8"/>
     </row>
-    <row r="551" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="551" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K551" s="8"/>
     </row>
-    <row r="552" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="552" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K552" s="8"/>
     </row>
-    <row r="553" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="553" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K553" s="8"/>
     </row>
-    <row r="554" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="554" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K554" s="8"/>
     </row>
-    <row r="555" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="555" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K555" s="8"/>
     </row>
-    <row r="556" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="556" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K556" s="8"/>
     </row>
-    <row r="557" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="557" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K557" s="8"/>
     </row>
-    <row r="558" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="558" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K558" s="8"/>
     </row>
-    <row r="559" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="559" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K559" s="8"/>
     </row>
-    <row r="560" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="560" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K560" s="8"/>
     </row>
-    <row r="561" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="561" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K561" s="8"/>
     </row>
-    <row r="562" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="562" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K562" s="8"/>
     </row>
-    <row r="563" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="563" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K563" s="8"/>
     </row>
-    <row r="564" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="564" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K564" s="8"/>
     </row>
-    <row r="565" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="565" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K565" s="8"/>
     </row>
-    <row r="566" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="566" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K566" s="8"/>
     </row>
-    <row r="567" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="567" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K567" s="8"/>
     </row>
-    <row r="568" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="568" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K568" s="8"/>
     </row>
-    <row r="569" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="569" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K569" s="8"/>
     </row>
-    <row r="570" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="570" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K570" s="8"/>
     </row>
-    <row r="571" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="571" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K571" s="8"/>
     </row>
-    <row r="572" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="572" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K572" s="8"/>
     </row>
-    <row r="573" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="573" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K573" s="8"/>
     </row>
-    <row r="574" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="574" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K574" s="8"/>
     </row>
-    <row r="575" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="575" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K575" s="8"/>
     </row>
-    <row r="576" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="576" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K576" s="8"/>
     </row>
-    <row r="577" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="577" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K577" s="8"/>
     </row>
-    <row r="578" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="578" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K578" s="8"/>
     </row>
-    <row r="579" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="579" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K579" s="8"/>
     </row>
-    <row r="580" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="580" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K580" s="8"/>
     </row>
-    <row r="581" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="581" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K581" s="8"/>
     </row>
-    <row r="582" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="582" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K582" s="8"/>
     </row>
-    <row r="583" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="583" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K583" s="8"/>
     </row>
-    <row r="584" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="584" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K584" s="8"/>
     </row>
-    <row r="585" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="585" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K585" s="8"/>
     </row>
-    <row r="586" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="586" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K586" s="8"/>
     </row>
-    <row r="587" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="587" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K587" s="8"/>
     </row>
-    <row r="588" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="588" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K588" s="8"/>
     </row>
-    <row r="589" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="589" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K589" s="8"/>
     </row>
-    <row r="590" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="590" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K590" s="8"/>
     </row>
-    <row r="591" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="591" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K591" s="8"/>
     </row>
-    <row r="592" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="592" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K592" s="8"/>
     </row>
-    <row r="593" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="593" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K593" s="8"/>
     </row>
-    <row r="594" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="594" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K594" s="8"/>
     </row>
-    <row r="595" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="595" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K595" s="8"/>
     </row>
-    <row r="596" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="596" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K596" s="8"/>
     </row>
-    <row r="597" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="597" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K597" s="8"/>
     </row>
-    <row r="598" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="598" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K598" s="8"/>
     </row>
-    <row r="599" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="599" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K599" s="8"/>
     </row>
-    <row r="600" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="600" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K600" s="8"/>
     </row>
-    <row r="601" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="601" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K601" s="8"/>
     </row>
-    <row r="602" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="602" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K602" s="8"/>
     </row>
-    <row r="603" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="603" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K603" s="8"/>
     </row>
-    <row r="604" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="604" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K604" s="8"/>
     </row>
-    <row r="605" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="605" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K605" s="8"/>
     </row>
-    <row r="606" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="606" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K606" s="8"/>
     </row>
-    <row r="607" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="607" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K607" s="8"/>
     </row>
-    <row r="608" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="608" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K608" s="8"/>
     </row>
-    <row r="609" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="609" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K609" s="8"/>
     </row>
-    <row r="610" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="610" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K610" s="8"/>
     </row>
-    <row r="611" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="611" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K611" s="8"/>
     </row>
-    <row r="612" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="612" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K612" s="8"/>
     </row>
-    <row r="613" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="613" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K613" s="8"/>
     </row>
-    <row r="614" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="614" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K614" s="8"/>
     </row>
-    <row r="615" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="615" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K615" s="8"/>
     </row>
-    <row r="616" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="616" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K616" s="8"/>
     </row>
-    <row r="617" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="617" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K617" s="8"/>
     </row>
-    <row r="618" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="618" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K618" s="8"/>
     </row>
-    <row r="619" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="619" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K619" s="8"/>
     </row>
-    <row r="620" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="620" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K620" s="8"/>
     </row>
-    <row r="621" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="621" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K621" s="8"/>
     </row>
-    <row r="622" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="622" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K622" s="8"/>
     </row>
-    <row r="623" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="623" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K623" s="8"/>
     </row>
-    <row r="624" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="624" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K624" s="8"/>
     </row>
-    <row r="625" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="625" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K625" s="8"/>
     </row>
-    <row r="626" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="626" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K626" s="8"/>
     </row>
-    <row r="627" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="627" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K627" s="8"/>
     </row>
-    <row r="628" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="628" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K628" s="8"/>
     </row>
-    <row r="629" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="629" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K629" s="8"/>
     </row>
-    <row r="630" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="630" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K630" s="8"/>
     </row>
-    <row r="631" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="631" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K631" s="8"/>
     </row>
-    <row r="632" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="632" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K632" s="8"/>
     </row>
-    <row r="633" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="633" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K633" s="8"/>
     </row>
-    <row r="634" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="634" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K634" s="8"/>
     </row>
-    <row r="635" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="635" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K635" s="8"/>
     </row>
-    <row r="636" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="636" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K636" s="8"/>
     </row>
-    <row r="637" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="637" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K637" s="8"/>
     </row>
-    <row r="638" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="638" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K638" s="8"/>
     </row>
-    <row r="639" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="639" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K639" s="8"/>
     </row>
-    <row r="640" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="640" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K640" s="8"/>
     </row>
-    <row r="641" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="641" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K641" s="8"/>
     </row>
-    <row r="642" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="642" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K642" s="8"/>
     </row>
-    <row r="643" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="643" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K643" s="8"/>
     </row>
-    <row r="644" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="644" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K644" s="8"/>
     </row>
-    <row r="645" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="645" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K645" s="8"/>
     </row>
-    <row r="646" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="646" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K646" s="8"/>
     </row>
-    <row r="647" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="647" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K647" s="8"/>
     </row>
-    <row r="648" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="648" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K648" s="8"/>
     </row>
-    <row r="649" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="649" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K649" s="8"/>
     </row>
-    <row r="650" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="650" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K650" s="8"/>
     </row>
-    <row r="651" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="651" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K651" s="8"/>
     </row>
-    <row r="652" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="652" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K652" s="8"/>
     </row>
-    <row r="653" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="653" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K653" s="8"/>
     </row>
-    <row r="654" spans="11:11" x14ac:dyDescent="0.35">
+    <row r="654" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K654" s="8"/>
     </row>
   </sheetData>

</xml_diff>